<commit_message>
Graficos holt winters predicciones y valor real
</commit_message>
<xml_diff>
--- a/src/datos/metricas_holt_winters.xlsx
+++ b/src/datos/metricas_holt_winters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="569" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="310">
   <si>
     <t>MAPE</t>
   </si>
@@ -1363,16 +1363,16 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.3724244915904331</v>
+        <v>0.4786159257405775</v>
       </c>
       <c r="C4">
-        <v>0.5126389762545326</v>
+        <v>0.755022390658761</v>
       </c>
       <c r="D4">
-        <v>0.473017229426453</v>
+        <v>0.5700361977484854</v>
       </c>
       <c r="E4">
-        <v>0.2627987199752952</v>
+        <v>0.5700588103960708</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -1397,16 +1397,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>0.3469605189118105</v>
+        <v>0.4545563968782935</v>
       </c>
       <c r="C6">
-        <v>0.631835637857912</v>
+        <v>0.6634263868417892</v>
       </c>
       <c r="D6">
-        <v>0.4960712972590511</v>
+        <v>0.5680840767845996</v>
       </c>
       <c r="E6">
-        <v>0.3992162732673145</v>
+        <v>0.4401345707579514</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -1431,16 +1431,16 @@
         <v>11</v>
       </c>
       <c r="B8">
-        <v>0.272918764553892</v>
+        <v>0.2670677692760683</v>
       </c>
       <c r="C8">
-        <v>1.615711983309445</v>
+        <v>1.612165698570702</v>
       </c>
       <c r="D8">
-        <v>1.184886804332781</v>
+        <v>1.139560924801655</v>
       </c>
       <c r="E8">
-        <v>2.610525213009741</v>
+        <v>2.599078239647959</v>
       </c>
     </row>
     <row r="9" spans="1:5">
@@ -1482,16 +1482,16 @@
         <v>14</v>
       </c>
       <c r="B11">
-        <v>0.2543133834439815</v>
+        <v>0.2549249220838762</v>
       </c>
       <c r="C11">
-        <v>0.4920564998089503</v>
+        <v>0.4906077841478587</v>
       </c>
       <c r="D11">
-        <v>0.3742350072707807</v>
+        <v>0.3719962135281813</v>
       </c>
       <c r="E11">
-        <v>0.2421195990042355</v>
+        <v>0.2406959978664719</v>
       </c>
     </row>
     <row r="12" spans="1:5">
@@ -1499,16 +1499,16 @@
         <v>15</v>
       </c>
       <c r="B12">
-        <v>0.2148430819325764</v>
+        <v>0.2147783275441034</v>
       </c>
       <c r="C12">
-        <v>0.4649804020768866</v>
+        <v>0.4640992521149756</v>
       </c>
       <c r="D12">
-        <v>0.4296861638651528</v>
+        <v>0.4295566550882067</v>
       </c>
       <c r="E12">
-        <v>0.2162067743155831</v>
+        <v>0.2153881158136797</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -1516,16 +1516,16 @@
         <v>16</v>
       </c>
       <c r="B13">
-        <v>0.4971892184275973</v>
+        <v>0.4968978471534317</v>
       </c>
       <c r="C13">
-        <v>0.7033197079996117</v>
+        <v>0.7032482182362473</v>
       </c>
       <c r="D13">
-        <v>0.666874207262686</v>
+        <v>0.6684376609407851</v>
       </c>
       <c r="E13">
-        <v>0.4946586116606591</v>
+        <v>0.4945580564524565</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -1533,16 +1533,16 @@
         <v>17</v>
       </c>
       <c r="B14">
-        <v>0.8670772808566777</v>
+        <v>0.9319451154438096</v>
       </c>
       <c r="C14">
-        <v>2.590713313795646</v>
+        <v>2.389910218618248</v>
       </c>
       <c r="D14">
-        <v>1.898862790520261</v>
+        <v>1.907599413328976</v>
       </c>
       <c r="E14">
-        <v>6.711795474278019</v>
+        <v>5.711670853055924</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -1635,16 +1635,16 @@
         <v>23</v>
       </c>
       <c r="B20">
-        <v>0.3561215019686951</v>
+        <v>0.3221624661811275</v>
       </c>
       <c r="C20">
-        <v>0.5537167561444596</v>
+        <v>0.6255051020963646</v>
       </c>
       <c r="D20">
-        <v>0.469535298804305</v>
+        <v>0.4581811564381348</v>
       </c>
       <c r="E20">
-        <v>0.306602246035143</v>
+        <v>0.3912566327485835</v>
       </c>
     </row>
     <row r="21" spans="1:5">
@@ -1686,16 +1686,16 @@
         <v>26</v>
       </c>
       <c r="B23">
-        <v>0.1211108042020731</v>
+        <v>0.1310435745345375</v>
       </c>
       <c r="C23">
-        <v>2.042648955384926</v>
+        <v>2.075470625285276</v>
       </c>
       <c r="D23">
-        <v>1.771932259559478</v>
+        <v>1.878490367943796</v>
       </c>
       <c r="E23">
-        <v>4.172414754935128</v>
+        <v>4.307578316422056</v>
       </c>
     </row>
     <row r="24" spans="1:5">
@@ -1703,16 +1703,16 @@
         <v>27</v>
       </c>
       <c r="B24">
-        <v>0.6969109047654308</v>
+        <v>0.557084793290984</v>
       </c>
       <c r="C24">
-        <v>1.537784599910478</v>
+        <v>1.067099398783278</v>
       </c>
       <c r="D24">
-        <v>1.198071401321856</v>
+        <v>0.9032247540237153</v>
       </c>
       <c r="E24">
-        <v>2.364781475721828</v>
+        <v>1.138701126883633</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -1720,16 +1720,16 @@
         <v>28</v>
       </c>
       <c r="B25">
-        <v>0.1314267257015177</v>
+        <v>0.1307600912201932</v>
       </c>
       <c r="C25">
-        <v>0.4716113687236588</v>
+        <v>0.4733439640348152</v>
       </c>
       <c r="D25">
-        <v>0.2492328940378395</v>
+        <v>0.249022041882536</v>
       </c>
       <c r="E25">
-        <v>0.2224172831094028</v>
+        <v>0.2240545082881924</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -1771,16 +1771,16 @@
         <v>31</v>
       </c>
       <c r="B28">
-        <v>0.3437590882186086</v>
+        <v>0.3437381795211782</v>
       </c>
       <c r="C28">
-        <v>0.4330236748913919</v>
+        <v>0.4330189520419868</v>
       </c>
       <c r="D28">
-        <v>0.3750122165683051</v>
+        <v>0.3749834207797675</v>
       </c>
       <c r="E28">
-        <v>0.1875095030164459</v>
+        <v>0.1875054128275405</v>
       </c>
     </row>
     <row r="29" spans="1:5">
@@ -1839,16 +1839,16 @@
         <v>35</v>
       </c>
       <c r="B32">
-        <v>0.3493780669233906</v>
+        <v>0.3200363007370892</v>
       </c>
       <c r="C32">
-        <v>0.6611661438083687</v>
+        <v>0.5235452232364999</v>
       </c>
       <c r="D32">
-        <v>0.4723630605203193</v>
+        <v>0.4360728874094498</v>
       </c>
       <c r="E32">
-        <v>0.4371406697184284</v>
+        <v>0.2740996007737564</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -1856,16 +1856,16 @@
         <v>36</v>
       </c>
       <c r="B33">
-        <v>0.3149180229258025</v>
+        <v>0.3145204465430077</v>
       </c>
       <c r="C33">
-        <v>0.6017976723748384</v>
+        <v>0.6008742914737856</v>
       </c>
       <c r="D33">
-        <v>0.4154425992028765</v>
+        <v>0.4152640847500993</v>
       </c>
       <c r="E33">
-        <v>0.3621604384757733</v>
+        <v>0.3610499141541238</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -1890,16 +1890,16 @@
         <v>38</v>
       </c>
       <c r="B35">
-        <v>0.496528740340938</v>
+        <v>0.6795331134144447</v>
       </c>
       <c r="C35">
-        <v>1.06053662508337</v>
+        <v>1.325851756907938</v>
       </c>
       <c r="D35">
-        <v>0.9030934895854547</v>
+        <v>1.075602446153669</v>
       </c>
       <c r="E35">
-        <v>1.124737933143225</v>
+        <v>1.757882881295865</v>
       </c>
     </row>
     <row r="36" spans="1:5">
@@ -1907,16 +1907,16 @@
         <v>39</v>
       </c>
       <c r="B36">
-        <v>0.4954629190080993</v>
+        <v>0.4890287721415538</v>
       </c>
       <c r="C36">
-        <v>0.9078153321855861</v>
+        <v>0.9079001531611948</v>
       </c>
       <c r="D36">
-        <v>0.7735260570003507</v>
+        <v>0.7739171316611608</v>
       </c>
       <c r="E36">
-        <v>0.8241286773512261</v>
+        <v>0.824282688110121</v>
       </c>
     </row>
     <row r="37" spans="1:5">
@@ -1924,16 +1924,16 @@
         <v>40</v>
       </c>
       <c r="B37">
-        <v>0.5776091633873334</v>
+        <v>0.5575769245209362</v>
       </c>
       <c r="C37">
-        <v>1.134953317796741</v>
+        <v>1.077150542713417</v>
       </c>
       <c r="D37">
-        <v>0.941527334867737</v>
+        <v>0.8998047072740362</v>
       </c>
       <c r="E37">
-        <v>1.288119033577829</v>
+        <v>1.160253291667808</v>
       </c>
     </row>
     <row r="38" spans="1:5">
@@ -1992,16 +1992,16 @@
         <v>44</v>
       </c>
       <c r="B41">
-        <v>0.3734763072717564</v>
+        <v>0.3665698056508733</v>
       </c>
       <c r="C41">
-        <v>0.632240040222893</v>
+        <v>0.5376426344668498</v>
       </c>
       <c r="D41">
-        <v>0.4832377682675771</v>
+        <v>0.4873440226703996</v>
       </c>
       <c r="E41">
-        <v>0.3997274684610454</v>
+        <v>0.2890596023964546</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -2145,16 +2145,16 @@
         <v>53</v>
       </c>
       <c r="B50">
-        <v>0.4219054946240982</v>
+        <v>0.4731759496831794</v>
       </c>
       <c r="C50">
-        <v>0.853672424871913</v>
+        <v>1.020650614984815</v>
       </c>
       <c r="D50">
-        <v>0.687848524850297</v>
+        <v>0.7678848446471102</v>
       </c>
       <c r="E50">
-        <v>0.7287566089866919</v>
+        <v>1.041727677868882</v>
       </c>
     </row>
     <row r="51" spans="1:5">
@@ -2162,16 +2162,16 @@
         <v>54</v>
       </c>
       <c r="B51">
-        <v>0.3090740306663173</v>
+        <v>0.2797544763591776</v>
       </c>
       <c r="C51">
-        <v>0.6375010864415384</v>
+        <v>0.4685180829856558</v>
       </c>
       <c r="D51">
-        <v>0.4518318638882261</v>
+        <v>0.3869346330242098</v>
       </c>
       <c r="E51">
-        <v>0.4064076352141417</v>
+        <v>0.2195091940845539</v>
       </c>
     </row>
     <row r="52" spans="1:5">
@@ -2230,16 +2230,16 @@
         <v>58</v>
       </c>
       <c r="B55">
-        <v>0.2725757621948275</v>
+        <v>0.2728717814779802</v>
       </c>
       <c r="C55">
-        <v>0.5961205390039332</v>
+        <v>0.5962388409888273</v>
       </c>
       <c r="D55">
-        <v>0.3908272794459358</v>
+        <v>0.391176140207442</v>
       </c>
       <c r="E55">
-        <v>0.3553596970223399</v>
+        <v>0.3555007555037001</v>
       </c>
     </row>
     <row r="56" spans="1:5">
@@ -2315,16 +2315,16 @@
         <v>63</v>
       </c>
       <c r="B60">
-        <v>0.2903971471010123</v>
+        <v>0.2673696251160489</v>
       </c>
       <c r="C60">
-        <v>0.5247411156339202</v>
+        <v>0.5327323147308363</v>
       </c>
       <c r="D60">
-        <v>0.3990261182946844</v>
+        <v>0.3853519397292767</v>
       </c>
       <c r="E60">
-        <v>0.2753532384367312</v>
+        <v>0.2838037191584748</v>
       </c>
     </row>
     <row r="61" spans="1:5">
@@ -2332,16 +2332,16 @@
         <v>64</v>
       </c>
       <c r="B61">
-        <v>0.3536831426165967</v>
+        <v>0.3473245181312337</v>
       </c>
       <c r="C61">
-        <v>0.6768812766850703</v>
+        <v>0.678739671753805</v>
       </c>
       <c r="D61">
-        <v>0.4754495737107338</v>
+        <v>0.470466955885778</v>
       </c>
       <c r="E61">
-        <v>0.4581682627268107</v>
+        <v>0.460687542012463</v>
       </c>
     </row>
     <row r="62" spans="1:5">
@@ -2349,16 +2349,16 @@
         <v>65</v>
       </c>
       <c r="B62">
-        <v>0.3872994555676597</v>
+        <v>0.3615238687196522</v>
       </c>
       <c r="C62">
-        <v>0.5561702856762729</v>
+        <v>0.5536541842518955</v>
       </c>
       <c r="D62">
-        <v>0.4670359521269522</v>
+        <v>0.4479461011349036</v>
       </c>
       <c r="E62">
-        <v>0.309325386669227</v>
+        <v>0.3065329557396319</v>
       </c>
     </row>
     <row r="63" spans="1:5">
@@ -2383,16 +2383,16 @@
         <v>67</v>
       </c>
       <c r="B64">
-        <v>0.4275530837213884</v>
+        <v>0.4157794459197763</v>
       </c>
       <c r="C64">
-        <v>0.7054352963797141</v>
+        <v>0.6658851851783817</v>
       </c>
       <c r="D64">
-        <v>0.5347784336038821</v>
+        <v>0.5261323580908888</v>
       </c>
       <c r="E64">
-        <v>0.4976389573783352</v>
+        <v>0.4434030798400477</v>
       </c>
     </row>
     <row r="65" spans="1:5">
@@ -2468,16 +2468,16 @@
         <v>72</v>
       </c>
       <c r="B69">
-        <v>0.40781137109793</v>
+        <v>0.4244734567353318</v>
       </c>
       <c r="C69">
-        <v>0.7067804554644428</v>
+        <v>0.6550313125707917</v>
       </c>
       <c r="D69">
-        <v>0.513725088023647</v>
+        <v>0.5183609446666377</v>
       </c>
       <c r="E69">
-        <v>0.4995386122265251</v>
+        <v>0.4290660204482142</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -2536,16 +2536,16 @@
         <v>76</v>
       </c>
       <c r="B73">
-        <v>0.2352805848277945</v>
+        <v>0.2302740088263384</v>
       </c>
       <c r="C73">
-        <v>0.5246520284148298</v>
+        <v>0.5546221682165207</v>
       </c>
       <c r="D73">
-        <v>0.3778092504347382</v>
+        <v>0.3818657285338691</v>
       </c>
       <c r="E73">
-        <v>0.2752597509197954</v>
+        <v>0.3076057494771945</v>
       </c>
     </row>
     <row r="74" spans="1:5">
@@ -2553,16 +2553,16 @@
         <v>77</v>
       </c>
       <c r="B74">
-        <v>0.7400106019980003</v>
+        <v>0.7329971909884208</v>
       </c>
       <c r="C74">
-        <v>1.246086057470312</v>
+        <v>1.242631685611776</v>
       </c>
       <c r="D74">
-        <v>1.043945695715472</v>
+        <v>1.039363984253922</v>
       </c>
       <c r="E74">
-        <v>1.552730462621906</v>
+        <v>1.544133506086363</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -2587,16 +2587,16 @@
         <v>79</v>
       </c>
       <c r="B76">
-        <v>0.4452260358790869</v>
+        <v>0.5358402206237433</v>
       </c>
       <c r="C76">
-        <v>0.5209020756713323</v>
+        <v>0.7650529275874877</v>
       </c>
       <c r="D76">
-        <v>0.5166221354885077</v>
+        <v>0.5966267425561554</v>
       </c>
       <c r="E76">
-        <v>0.2713389724387024</v>
+        <v>0.5853059820101856</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -2638,16 +2638,16 @@
         <v>82</v>
       </c>
       <c r="B79">
-        <v>0.3169919717358239</v>
+        <v>0.3447889400469858</v>
       </c>
       <c r="C79">
-        <v>0.4912656680809127</v>
+        <v>0.4899529607784295</v>
       </c>
       <c r="D79">
-        <v>0.4428051482877731</v>
+        <v>0.4598969363494763</v>
       </c>
       <c r="E79">
-        <v>0.2413419566349855</v>
+        <v>0.2400539037755493</v>
       </c>
     </row>
     <row r="80" spans="1:5">
@@ -2689,16 +2689,16 @@
         <v>85</v>
       </c>
       <c r="B82">
-        <v>0.3273996486257328</v>
+        <v>0.3275668615251359</v>
       </c>
       <c r="C82">
-        <v>0.5221388293212799</v>
+        <v>0.5236156303002666</v>
       </c>
       <c r="D82">
-        <v>0.4625667264269865</v>
+        <v>0.4606941998367151</v>
       </c>
       <c r="E82">
-        <v>0.2726289570849967</v>
+        <v>0.2741733282947454</v>
       </c>
     </row>
     <row r="83" spans="1:5">
@@ -2706,16 +2706,16 @@
         <v>86</v>
       </c>
       <c r="B83">
-        <v>0.3988872738534948</v>
+        <v>0.3898210422961594</v>
       </c>
       <c r="C83">
-        <v>0.7105947265229046</v>
+        <v>0.7087395793297024</v>
       </c>
       <c r="D83">
-        <v>0.5223490885744645</v>
+        <v>0.5143996053857582</v>
       </c>
       <c r="E83">
-        <v>0.5049448653621615</v>
+        <v>0.5023117913084435</v>
       </c>
     </row>
     <row r="84" spans="1:5">
@@ -2791,16 +2791,16 @@
         <v>91</v>
       </c>
       <c r="B88">
-        <v>0.4254124558906757</v>
+        <v>0.3812197986247686</v>
       </c>
       <c r="C88">
-        <v>0.6585445732139241</v>
+        <v>0.6366712361617799</v>
       </c>
       <c r="D88">
-        <v>0.6060579816401841</v>
+        <v>0.5825230689459123</v>
       </c>
       <c r="E88">
-        <v>0.4336809549095094</v>
+        <v>0.4053502629557689</v>
       </c>
     </row>
     <row r="89" spans="1:5">
@@ -2859,16 +2859,16 @@
         <v>95</v>
       </c>
       <c r="B92">
-        <v>0.4407260032941415</v>
+        <v>0.2842057951834712</v>
       </c>
       <c r="C92">
-        <v>0.7150206542961758</v>
+        <v>0.4682721821337013</v>
       </c>
       <c r="D92">
-        <v>0.5309856384389163</v>
+        <v>0.3998343470679004</v>
       </c>
       <c r="E92">
-        <v>0.5112545360701313</v>
+        <v>0.2192788365602583</v>
       </c>
     </row>
     <row r="93" spans="1:5">
@@ -2876,16 +2876,16 @@
         <v>96</v>
       </c>
       <c r="B93">
-        <v>0.8619703026556494</v>
+        <v>0.8616530478472439</v>
       </c>
       <c r="C93">
-        <v>1.066694749894717</v>
+        <v>1.067079801677238</v>
       </c>
       <c r="D93">
-        <v>0.9414343305032588</v>
+        <v>0.9416693633842241</v>
       </c>
       <c r="E93">
-        <v>1.137837689452952</v>
+        <v>1.138659303147533</v>
       </c>
     </row>
     <row r="94" spans="1:5">
@@ -2927,16 +2927,16 @@
         <v>99</v>
       </c>
       <c r="B96">
-        <v>0.219602531000217</v>
+        <v>0.2019114778355784</v>
       </c>
       <c r="C96">
-        <v>0.3728304432810467</v>
+        <v>0.3342987036526547</v>
       </c>
       <c r="D96">
-        <v>0.3018942773963259</v>
+        <v>0.2928254318398145</v>
       </c>
       <c r="E96">
-        <v>0.1390025394371418</v>
+        <v>0.1117556232638455</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -2944,16 +2944,16 @@
         <v>100</v>
       </c>
       <c r="B97">
-        <v>0.343202042173766</v>
+        <v>0.3306115385024645</v>
       </c>
       <c r="C97">
-        <v>0.5237532510799557</v>
+        <v>0.5127650056510681</v>
       </c>
       <c r="D97">
-        <v>0.4367029779373194</v>
+        <v>0.4166667265144413</v>
       </c>
       <c r="E97">
-        <v>0.2743174680168231</v>
+        <v>0.2629279510203399</v>
       </c>
     </row>
     <row r="98" spans="1:5">
@@ -2961,16 +2961,16 @@
         <v>101</v>
       </c>
       <c r="B98">
-        <v>0.04050973865783754</v>
+        <v>0.04047032321572885</v>
       </c>
       <c r="C98">
-        <v>0.09819853161228308</v>
+        <v>0.09796118427446869</v>
       </c>
       <c r="D98">
-        <v>0.0981005404339288</v>
+        <v>0.09788766860147491</v>
       </c>
       <c r="E98">
-        <v>0.009642951610808559</v>
+        <v>0.009596393624456412</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -2978,16 +2978,16 @@
         <v>102</v>
       </c>
       <c r="B99">
-        <v>0.425814601599825</v>
+        <v>0.4031848021034972</v>
       </c>
       <c r="C99">
-        <v>0.5980061807207706</v>
+        <v>0.6004906711086188</v>
       </c>
       <c r="D99">
-        <v>0.5364873672957843</v>
+        <v>0.5274945977223285</v>
       </c>
       <c r="E99">
-        <v>0.357611392180243</v>
+        <v>0.3605890460884794</v>
       </c>
     </row>
     <row r="100" spans="1:5">
@@ -3011,17 +3011,17 @@
       <c r="A101" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="B101">
-        <v>0.6525689048486183</v>
-      </c>
-      <c r="C101">
-        <v>1.230874415449621</v>
-      </c>
-      <c r="D101">
-        <v>1.024353623299346</v>
-      </c>
-      <c r="E101">
-        <v>1.515051826608446</v>
+      <c r="B101" t="s">
+        <v>309</v>
+      </c>
+      <c r="C101" t="s">
+        <v>309</v>
+      </c>
+      <c r="D101" t="s">
+        <v>309</v>
+      </c>
+      <c r="E101" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="102" spans="1:5">
@@ -3029,16 +3029,16 @@
         <v>105</v>
       </c>
       <c r="B102">
-        <v>0.4259401573732943</v>
+        <v>0.4437562788181308</v>
       </c>
       <c r="C102">
-        <v>0.6521595277853565</v>
+        <v>0.5419410017371094</v>
       </c>
       <c r="D102">
-        <v>0.5253886897224062</v>
+        <v>0.5215317451020389</v>
       </c>
       <c r="E102">
-        <v>0.4253120496812192</v>
+        <v>0.2937000493638215</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -3046,16 +3046,16 @@
         <v>106</v>
       </c>
       <c r="B103">
-        <v>0.5041608550659019</v>
+        <v>0.4266131580124726</v>
       </c>
       <c r="C103">
-        <v>0.9174656313417737</v>
+        <v>0.828176042756941</v>
       </c>
       <c r="D103">
-        <v>0.7722885237479612</v>
+        <v>0.7124180524816969</v>
       </c>
       <c r="E103">
-        <v>0.8417431846933595</v>
+        <v>0.6858755577965466</v>
       </c>
     </row>
     <row r="104" spans="1:5">
@@ -3165,16 +3165,16 @@
         <v>113</v>
       </c>
       <c r="B110">
-        <v>0.5703276261821977</v>
+        <v>0.5606703967573561</v>
       </c>
       <c r="C110">
-        <v>1.085633408557752</v>
+        <v>1.094787250557016</v>
       </c>
       <c r="D110">
-        <v>0.9688681304428483</v>
+        <v>0.9871534895551436</v>
       </c>
       <c r="E110">
-        <v>1.178599897776723</v>
+        <v>1.19855912398219</v>
       </c>
     </row>
     <row r="111" spans="1:5">
@@ -3182,16 +3182,16 @@
         <v>114</v>
       </c>
       <c r="B111">
-        <v>0.4436410775229312</v>
+        <v>0.4377258474238803</v>
       </c>
       <c r="C111">
-        <v>0.6590105995594276</v>
+        <v>0.6608588427786001</v>
       </c>
       <c r="D111">
-        <v>0.593482486361359</v>
+        <v>0.5795358058210212</v>
       </c>
       <c r="E111">
-        <v>0.4342949703316762</v>
+        <v>0.4367344100786704</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -3199,16 +3199,16 @@
         <v>115</v>
       </c>
       <c r="B112">
-        <v>0.8461433996245656</v>
+        <v>0.8277268435390726</v>
       </c>
       <c r="C112">
-        <v>1.573993508453883</v>
+        <v>1.564701621374149</v>
       </c>
       <c r="D112">
-        <v>1.253847826719042</v>
+        <v>1.197629677473109</v>
       </c>
       <c r="E112">
-        <v>2.477455564654963</v>
+        <v>2.448291163930891</v>
       </c>
     </row>
     <row r="113" spans="1:5">
@@ -3301,16 +3301,16 @@
         <v>121</v>
       </c>
       <c r="B118">
-        <v>0.4014330590159637</v>
+        <v>0.4015443501172283</v>
       </c>
       <c r="C118">
-        <v>0.6932732057181037</v>
+        <v>0.6911523530306445</v>
       </c>
       <c r="D118">
-        <v>0.5313321203941098</v>
+        <v>0.5336916550811015</v>
       </c>
       <c r="E118">
-        <v>0.4806277377666561</v>
+        <v>0.4776915750997966</v>
       </c>
     </row>
     <row r="119" spans="1:5">
@@ -3318,16 +3318,16 @@
         <v>122</v>
       </c>
       <c r="B119">
-        <v>0.3322655185567899</v>
+        <v>0.337358947745595</v>
       </c>
       <c r="C119">
-        <v>0.5668563594760111</v>
+        <v>0.5924437073980731</v>
       </c>
       <c r="D119">
-        <v>0.4661223907453375</v>
+        <v>0.4473545044725566</v>
       </c>
       <c r="E119">
-        <v>0.3213261322783967</v>
+        <v>0.3509895464355737</v>
       </c>
     </row>
     <row r="120" spans="1:5">
@@ -3335,33 +3335,33 @@
         <v>123</v>
       </c>
       <c r="B120">
-        <v>0.5303007526675569</v>
+        <v>0.5125098216031823</v>
       </c>
       <c r="C120">
-        <v>1.057998826057126</v>
+        <v>0.8512603564830878</v>
       </c>
       <c r="D120">
-        <v>0.867365847959175</v>
+        <v>0.7098522362197364</v>
       </c>
       <c r="E120">
-        <v>1.119361515938256</v>
+        <v>0.7246441945197138</v>
       </c>
     </row>
     <row r="121" spans="1:5">
       <c r="A121" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B121" t="s">
-        <v>309</v>
-      </c>
-      <c r="C121" t="s">
-        <v>309</v>
-      </c>
-      <c r="D121" t="s">
-        <v>309</v>
-      </c>
-      <c r="E121" t="s">
-        <v>309</v>
+      <c r="B121">
+        <v>0.4397933416802167</v>
+      </c>
+      <c r="C121">
+        <v>0.671079921099928</v>
+      </c>
+      <c r="D121">
+        <v>0.54730763372631</v>
+      </c>
+      <c r="E121">
+        <v>0.4503482605034855</v>
       </c>
     </row>
     <row r="122" spans="1:5">
@@ -3369,16 +3369,16 @@
         <v>125</v>
       </c>
       <c r="B122">
-        <v>0.4802521659502891</v>
+        <v>0.4313772339696184</v>
       </c>
       <c r="C122">
-        <v>0.7053204028544465</v>
+        <v>0.7047093069086596</v>
       </c>
       <c r="D122">
-        <v>0.6178999849786216</v>
+        <v>0.5986494409869795</v>
       </c>
       <c r="E122">
-        <v>0.4974768706827588</v>
+        <v>0.4966152072436835</v>
       </c>
     </row>
     <row r="123" spans="1:5">
@@ -3386,16 +3386,16 @@
         <v>126</v>
       </c>
       <c r="B123">
-        <v>0.6472861163085062</v>
+        <v>0.6404930472911458</v>
       </c>
       <c r="C123">
-        <v>1.333769613441986</v>
+        <v>1.373693740113043</v>
       </c>
       <c r="D123">
-        <v>1.121431801415202</v>
+        <v>1.127505269894987</v>
       </c>
       <c r="E123">
-        <v>1.778941381741184</v>
+        <v>1.887034491625761</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -3454,16 +3454,16 @@
         <v>130</v>
       </c>
       <c r="B127">
-        <v>0.2964250999605031</v>
+        <v>0.3028653102081582</v>
       </c>
       <c r="C127">
-        <v>0.5451190451751333</v>
+        <v>0.5469195220110861</v>
       </c>
       <c r="D127">
-        <v>0.4003250966672082</v>
+        <v>0.4058849539561075</v>
       </c>
       <c r="E127">
-        <v>0.2971547734126491</v>
+        <v>0.2991209635568349</v>
       </c>
     </row>
     <row r="128" spans="1:5">
@@ -3471,16 +3471,16 @@
         <v>131</v>
       </c>
       <c r="B128">
-        <v>0.3803525101055732</v>
+        <v>0.373749274962926</v>
       </c>
       <c r="C128">
-        <v>0.6637332221796745</v>
+        <v>0.642106173305999</v>
       </c>
       <c r="D128">
-        <v>0.4893022214843988</v>
+        <v>0.4713915755645671</v>
       </c>
       <c r="E128">
-        <v>0.4405417902250131</v>
+        <v>0.4123003377976736</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -3590,16 +3590,16 @@
         <v>138</v>
       </c>
       <c r="B135">
-        <v>0.06957667427521347</v>
+        <v>0.06982209872425914</v>
       </c>
       <c r="C135">
-        <v>1.12545404853139</v>
+        <v>1.112067819331729</v>
       </c>
       <c r="D135">
-        <v>0.8420540767029404</v>
+        <v>0.8473289813033918</v>
       </c>
       <c r="E135">
-        <v>1.266646815355696</v>
+        <v>1.236694834793227</v>
       </c>
     </row>
     <row r="136" spans="1:5">
@@ -3624,16 +3624,16 @@
         <v>140</v>
       </c>
       <c r="B137">
-        <v>0.2909716131441348</v>
+        <v>0.4078525557005931</v>
       </c>
       <c r="C137">
-        <v>0.6332991926428401</v>
+        <v>0.7063199155973439</v>
       </c>
       <c r="D137">
-        <v>0.4625536056782038</v>
+        <v>0.5161808777133077</v>
       </c>
       <c r="E137">
-        <v>0.401067867402073</v>
+        <v>0.498887823169439</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -3641,16 +3641,16 @@
         <v>141</v>
       </c>
       <c r="B138">
-        <v>0.394493061429427</v>
+        <v>0.4017635543975263</v>
       </c>
       <c r="C138">
-        <v>2.110990522960438</v>
+        <v>2.109896462756877</v>
       </c>
       <c r="D138">
-        <v>1.616640890016631</v>
+        <v>1.632171501383522</v>
       </c>
       <c r="E138">
-        <v>4.456280988028785</v>
+        <v>4.451663083553983</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -3658,16 +3658,16 @@
         <v>142</v>
       </c>
       <c r="B139">
-        <v>0.3470744334693286</v>
+        <v>0.3901185587949892</v>
       </c>
       <c r="C139">
-        <v>0.6028009877820211</v>
+        <v>0.6243205925041276</v>
       </c>
       <c r="D139">
-        <v>0.4942055942317459</v>
+        <v>0.5060811071523945</v>
       </c>
       <c r="E139">
-        <v>0.3633690308709804</v>
+        <v>0.3897762022247049</v>
       </c>
     </row>
     <row r="140" spans="1:5">
@@ -3675,16 +3675,16 @@
         <v>143</v>
       </c>
       <c r="B140">
-        <v>0.403486237385273</v>
+        <v>0.4159342962396649</v>
       </c>
       <c r="C140">
-        <v>0.5993497460465663</v>
+        <v>0.6081529508295201</v>
       </c>
       <c r="D140">
-        <v>0.4706413318749573</v>
+        <v>0.4820797921934959</v>
       </c>
       <c r="E140">
-        <v>0.3592201180860836</v>
+        <v>0.3698500116026528</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -3692,16 +3692,16 @@
         <v>144</v>
       </c>
       <c r="B141">
-        <v>0.2521074249319283</v>
+        <v>0.2635092883960503</v>
       </c>
       <c r="C141">
-        <v>0.3910362071423966</v>
+        <v>0.4019733918098995</v>
       </c>
       <c r="D141">
-        <v>0.288263463155257</v>
+        <v>0.3119576709163328</v>
       </c>
       <c r="E141">
-        <v>0.1529093152963113</v>
+        <v>0.161582607723155</v>
       </c>
     </row>
     <row r="142" spans="1:5">
@@ -3725,17 +3725,17 @@
       <c r="A143" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="B143" t="s">
-        <v>309</v>
-      </c>
-      <c r="C143" t="s">
-        <v>309</v>
-      </c>
-      <c r="D143" t="s">
-        <v>309</v>
-      </c>
-      <c r="E143" t="s">
-        <v>309</v>
+      <c r="B143">
+        <v>0.6531642331625053</v>
+      </c>
+      <c r="C143">
+        <v>1.223500864374444</v>
+      </c>
+      <c r="D143">
+        <v>0.9845106242974208</v>
+      </c>
+      <c r="E143">
+        <v>1.496954365125012</v>
       </c>
     </row>
     <row r="144" spans="1:5">
@@ -3743,16 +3743,16 @@
         <v>147</v>
       </c>
       <c r="B144">
-        <v>0.7089709282108241</v>
+        <v>0.631606891739697</v>
       </c>
       <c r="C144">
-        <v>1.222087654363379</v>
+        <v>0.9914245650828248</v>
       </c>
       <c r="D144">
-        <v>0.9859680522986576</v>
+        <v>0.8372127836212011</v>
       </c>
       <c r="E144">
-        <v>1.493498234947386</v>
+        <v>0.9829226682496685</v>
       </c>
     </row>
     <row r="145" spans="1:5">
@@ -3760,16 +3760,16 @@
         <v>148</v>
       </c>
       <c r="B145">
-        <v>0.2525016707454921</v>
+        <v>0.2504605990832094</v>
       </c>
       <c r="C145">
-        <v>0.5589342747452075</v>
+        <v>0.5589938348877533</v>
       </c>
       <c r="D145">
-        <v>0.3771284495251888</v>
+        <v>0.3753908754300346</v>
       </c>
       <c r="E145">
-        <v>0.3124075234849511</v>
+        <v>0.3124741074425169</v>
       </c>
     </row>
     <row r="146" spans="1:5">
@@ -3777,16 +3777,16 @@
         <v>149</v>
       </c>
       <c r="B146">
-        <v>0.34446002359523</v>
+        <v>0.4646639342262309</v>
       </c>
       <c r="C146">
-        <v>1.16446560891605</v>
+        <v>0.8958068068389419</v>
       </c>
       <c r="D146">
-        <v>0.8410211025944136</v>
+        <v>0.7381323599057443</v>
       </c>
       <c r="E146">
-        <v>1.355980154348227</v>
+        <v>0.8024698351789814</v>
       </c>
     </row>
     <row r="147" spans="1:5">
@@ -3794,16 +3794,16 @@
         <v>150</v>
       </c>
       <c r="B147">
-        <v>0.7725227741563006</v>
+        <v>0.6900082985386168</v>
       </c>
       <c r="C147">
-        <v>1.173530077139152</v>
+        <v>1.20176319288909</v>
       </c>
       <c r="D147">
-        <v>1.011542332123706</v>
+        <v>0.9896037013492284</v>
       </c>
       <c r="E147">
-        <v>1.377172841950223</v>
+        <v>1.444234771782979</v>
       </c>
     </row>
     <row r="148" spans="1:5">
@@ -3811,16 +3811,16 @@
         <v>151</v>
       </c>
       <c r="B148">
-        <v>1.0969713879088</v>
+        <v>1.097643735628091</v>
       </c>
       <c r="C148">
-        <v>3.33324883541388</v>
+        <v>3.324984530415471</v>
       </c>
       <c r="D148">
-        <v>2.552580516174844</v>
+        <v>2.556007399895719</v>
       </c>
       <c r="E148">
-        <v>11.11054779878799</v>
+        <v>11.05552212750219</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -3828,16 +3828,16 @@
         <v>152</v>
       </c>
       <c r="B149">
-        <v>0.4916311478341936</v>
+        <v>0.4918868138606089</v>
       </c>
       <c r="C149">
-        <v>0.9213065251794815</v>
+        <v>0.9212612028274402</v>
       </c>
       <c r="D149">
-        <v>0.7357970712923932</v>
+        <v>0.7359859820436623</v>
       </c>
       <c r="E149">
-        <v>0.8488057133382907</v>
+        <v>0.8487222038350618</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -3862,16 +3862,16 @@
         <v>154</v>
       </c>
       <c r="B151">
-        <v>0.002380631681051533</v>
+        <v>0.001231219664849218</v>
       </c>
       <c r="C151">
-        <v>0.006596498200545643</v>
+        <v>0.003047598488197199</v>
       </c>
       <c r="D151">
-        <v>0.006176662856479331</v>
+        <v>0.002656043200645719</v>
       </c>
       <c r="E151">
-        <v>4.35137885098019E-05</v>
+        <v>9.287856545261855E-06</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -3879,16 +3879,16 @@
         <v>155</v>
       </c>
       <c r="B152">
-        <v>0.4827690068431137</v>
+        <v>0.4998299773296095</v>
       </c>
       <c r="C152">
-        <v>0.7365896843665525</v>
+        <v>0.735572877067064</v>
       </c>
       <c r="D152">
-        <v>0.6296300643997259</v>
+        <v>0.6385094718281457</v>
       </c>
       <c r="E152">
-        <v>0.5425643631152174</v>
+        <v>0.541067457476718</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -3896,16 +3896,16 @@
         <v>156</v>
       </c>
       <c r="B153">
-        <v>0.8613713785208418</v>
+        <v>0.8660212929177762</v>
       </c>
       <c r="C153">
-        <v>1.027863935383077</v>
+        <v>1.023883632447199</v>
       </c>
       <c r="D153">
-        <v>1.027019153868713</v>
+        <v>1.021615009692174</v>
       </c>
       <c r="E153">
-        <v>1.056504269661187</v>
+        <v>1.048337692793271</v>
       </c>
     </row>
     <row r="154" spans="1:5">
@@ -3930,16 +3930,16 @@
         <v>158</v>
       </c>
       <c r="B155">
-        <v>0.491700339807513</v>
+        <v>0.4963921174487012</v>
       </c>
       <c r="C155">
-        <v>0.8467331696475318</v>
+        <v>0.8074846316517033</v>
       </c>
       <c r="D155">
-        <v>0.7406575939995796</v>
+        <v>0.6975008617814493</v>
       </c>
       <c r="E155">
-        <v>0.7169570605813559</v>
+        <v>0.6520314303536868</v>
       </c>
     </row>
     <row r="156" spans="1:5">
@@ -3947,16 +3947,16 @@
         <v>159</v>
       </c>
       <c r="B156">
-        <v>0.0276537829007831</v>
+        <v>0.03111821028682598</v>
       </c>
       <c r="C156">
-        <v>0.9029295719174891</v>
+        <v>0.9695765194737833</v>
       </c>
       <c r="D156">
-        <v>0.7331533325296634</v>
+        <v>0.8090617188013017</v>
       </c>
       <c r="E156">
-        <v>0.8152818118431001</v>
+        <v>0.9400786271148958</v>
       </c>
     </row>
     <row r="157" spans="1:5">
@@ -4015,16 +4015,16 @@
         <v>163</v>
       </c>
       <c r="B160">
-        <v>0.3345936909244903</v>
+        <v>0.3395738975876917</v>
       </c>
       <c r="C160">
-        <v>0.528904015862953</v>
+        <v>0.5416783179761832</v>
       </c>
       <c r="D160">
-        <v>0.4293148343297219</v>
+        <v>0.4370505802251454</v>
       </c>
       <c r="E160">
-        <v>0.2797394579959588</v>
+        <v>0.293415400165507</v>
       </c>
     </row>
     <row r="161" spans="1:5">
@@ -4032,16 +4032,16 @@
         <v>164</v>
       </c>
       <c r="B161">
-        <v>0.3620700204734103</v>
+        <v>0.3654016012770241</v>
       </c>
       <c r="C161">
-        <v>0.5889700875441652</v>
+        <v>0.4955217180224747</v>
       </c>
       <c r="D161">
-        <v>0.4846236193930932</v>
+        <v>0.4805256267748906</v>
       </c>
       <c r="E161">
-        <v>0.3468857640217817</v>
+        <v>0.2455417730319449</v>
       </c>
     </row>
     <row r="162" spans="1:5">
@@ -4049,16 +4049,16 @@
         <v>165</v>
       </c>
       <c r="B162">
-        <v>0.247615777327809</v>
+        <v>0.2887371563224251</v>
       </c>
       <c r="C162">
-        <v>0.5578128135278237</v>
+        <v>0.5627273009898481</v>
       </c>
       <c r="D162">
-        <v>0.3775042320117711</v>
+        <v>0.4126861299340114</v>
       </c>
       <c r="E162">
-        <v>0.3111551349358266</v>
+        <v>0.3166620152793192</v>
       </c>
     </row>
     <row r="163" spans="1:5">
@@ -4066,16 +4066,16 @@
         <v>166</v>
       </c>
       <c r="B163">
-        <v>0.1107470844098153</v>
+        <v>0.1214518856596105</v>
       </c>
       <c r="C163">
-        <v>0.3372262815258225</v>
+        <v>0.3430332725840373</v>
       </c>
       <c r="D163">
-        <v>0.2638741451785382</v>
+        <v>0.2866434947901233</v>
       </c>
       <c r="E163">
-        <v>0.1137215649517333</v>
+        <v>0.1176718260997144</v>
       </c>
     </row>
     <row r="164" spans="1:5">
@@ -4134,16 +4134,16 @@
         <v>170</v>
       </c>
       <c r="B167">
-        <v>0.329399384161852</v>
+        <v>0.269223715242215</v>
       </c>
       <c r="C167">
-        <v>0.5076229908204601</v>
+        <v>0.5186209291370858</v>
       </c>
       <c r="D167">
-        <v>0.4402398218368916</v>
+        <v>0.4181837054256511</v>
       </c>
       <c r="E167">
-        <v>0.257681100809509</v>
+        <v>0.2689676681390142</v>
       </c>
     </row>
     <row r="168" spans="1:5">
@@ -4185,16 +4185,16 @@
         <v>173</v>
       </c>
       <c r="B170">
-        <v>0.7649661808100211</v>
+        <v>0.6692208974707655</v>
       </c>
       <c r="C170">
-        <v>1.780050257085418</v>
+        <v>1.363982698531102</v>
       </c>
       <c r="D170">
-        <v>1.434226505984087</v>
+        <v>1.160091064777155</v>
       </c>
       <c r="E170">
-        <v>3.168578917749861</v>
+        <v>1.860448801892186</v>
       </c>
     </row>
     <row r="171" spans="1:5">
@@ -4202,16 +4202,16 @@
         <v>174</v>
       </c>
       <c r="B171">
-        <v>0.5682921414328647</v>
+        <v>0.5569790817130985</v>
       </c>
       <c r="C171">
-        <v>0.8970372372773877</v>
+        <v>0.9718869219250746</v>
       </c>
       <c r="D171">
-        <v>0.7702735409665968</v>
+        <v>0.8240127126226309</v>
       </c>
       <c r="E171">
-        <v>0.8046758050622485</v>
+        <v>0.9445641890089961</v>
       </c>
     </row>
     <row r="172" spans="1:5">
@@ -4219,16 +4219,16 @@
         <v>175</v>
       </c>
       <c r="B172">
-        <v>0.3218210881766673</v>
+        <v>0.2533422502049488</v>
       </c>
       <c r="C172">
-        <v>0.4337136201340132</v>
+        <v>0.4267239626473744</v>
       </c>
       <c r="D172">
-        <v>0.3976400095629597</v>
+        <v>0.3424217096894482</v>
       </c>
       <c r="E172">
-        <v>0.1881075042897511</v>
+        <v>0.1820933402974778</v>
       </c>
     </row>
     <row r="173" spans="1:5">
@@ -4270,16 +4270,16 @@
         <v>178</v>
       </c>
       <c r="B175">
-        <v>0.2976583205644625</v>
+        <v>0.2768021867437396</v>
       </c>
       <c r="C175">
-        <v>0.5982598548643623</v>
+        <v>0.5970942398614163</v>
       </c>
       <c r="D175">
-        <v>0.400798609250373</v>
+        <v>0.3805334493659083</v>
       </c>
       <c r="E175">
-        <v>0.3579148539423278</v>
+        <v>0.3565215312756826</v>
       </c>
     </row>
     <row r="176" spans="1:5">
@@ -4321,16 +4321,16 @@
         <v>181</v>
       </c>
       <c r="B178">
-        <v>0.2748588535132971</v>
+        <v>0.2436788223199502</v>
       </c>
       <c r="C178">
-        <v>0.5960024582042815</v>
+        <v>0.4349685006061635</v>
       </c>
       <c r="D178">
-        <v>0.4200866538407341</v>
+        <v>0.3435035669191529</v>
       </c>
       <c r="E178">
-        <v>0.3552189301855464</v>
+        <v>0.1891975965195741</v>
       </c>
     </row>
     <row r="179" spans="1:5">
@@ -4355,16 +4355,16 @@
         <v>183</v>
       </c>
       <c r="B180">
-        <v>0.4154932136530313</v>
+        <v>0.414322638194175</v>
       </c>
       <c r="C180">
-        <v>0.7609673976609815</v>
+        <v>0.7612122670860567</v>
       </c>
       <c r="D180">
-        <v>0.5841292636273885</v>
+        <v>0.5831643435728465</v>
       </c>
       <c r="E180">
-        <v>0.5790713803029264</v>
+        <v>0.5794441155622941</v>
       </c>
     </row>
     <row r="181" spans="1:5">
@@ -4372,16 +4372,16 @@
         <v>184</v>
       </c>
       <c r="B181">
-        <v>0.4429144096599056</v>
+        <v>0.6050730532271311</v>
       </c>
       <c r="C181">
-        <v>1.079891833438346</v>
+        <v>1.262928099792141</v>
       </c>
       <c r="D181">
-        <v>0.8680280597723404</v>
+        <v>1.055509401444454</v>
       </c>
       <c r="E181">
-        <v>1.166166371926833</v>
+        <v>1.594987385244589</v>
       </c>
     </row>
     <row r="182" spans="1:5">
@@ -4389,16 +4389,16 @@
         <v>185</v>
       </c>
       <c r="B182">
-        <v>0.1436665252221327</v>
+        <v>0.1466427323993126</v>
       </c>
       <c r="C182">
-        <v>0.2643058855374002</v>
+        <v>0.2643743373512618</v>
       </c>
       <c r="D182">
-        <v>0.2004234183069266</v>
+        <v>0.2015560884028025</v>
       </c>
       <c r="E182">
-        <v>0.0698576011297093</v>
+        <v>0.06989379024991878</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -4406,16 +4406,16 @@
         <v>186</v>
       </c>
       <c r="B183">
-        <v>0.2755692255686503</v>
+        <v>0.2717783080131687</v>
       </c>
       <c r="C183">
-        <v>0.4402171894080676</v>
+        <v>0.4398556837339371</v>
       </c>
       <c r="D183">
-        <v>0.3254400815348381</v>
+        <v>0.3207297532358476</v>
       </c>
       <c r="E183">
-        <v>0.1937911738503385</v>
+        <v>0.1934730225130493</v>
       </c>
     </row>
     <row r="184" spans="1:5">
@@ -4440,16 +4440,16 @@
         <v>188</v>
       </c>
       <c r="B185">
-        <v>0.2986248697558678</v>
+        <v>0.4659578176980733</v>
       </c>
       <c r="C185">
-        <v>0.4918171156744728</v>
+        <v>0.6965052038590771</v>
       </c>
       <c r="D185">
-        <v>0.3883924813416109</v>
+        <v>0.6078167121124581</v>
       </c>
       <c r="E185">
-        <v>0.2418840752703578</v>
+        <v>0.4851194990027745</v>
       </c>
     </row>
     <row r="186" spans="1:5">
@@ -4491,16 +4491,16 @@
         <v>191</v>
       </c>
       <c r="B188">
-        <v>0.2648728586460916</v>
+        <v>0.2199114723123126</v>
       </c>
       <c r="C188">
-        <v>0.5217486853177266</v>
+        <v>0.5834589190109116</v>
       </c>
       <c r="D188">
-        <v>0.3760753481742218</v>
+        <v>0.3404895401001668</v>
       </c>
       <c r="E188">
-        <v>0.272221690630776</v>
+        <v>0.3404243101733815</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -4508,16 +4508,16 @@
         <v>192</v>
       </c>
       <c r="B189">
-        <v>0.3956057358611584</v>
+        <v>0.3974388335959377</v>
       </c>
       <c r="C189">
-        <v>0.688676176775343</v>
+        <v>0.6848355233510458</v>
       </c>
       <c r="D189">
-        <v>0.5014703002643667</v>
+        <v>0.5075545787844767</v>
       </c>
       <c r="E189">
-        <v>0.4742748764579034</v>
+        <v>0.4689996940435008</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -4525,16 +4525,16 @@
         <v>193</v>
       </c>
       <c r="B190">
-        <v>0.5017840392678836</v>
+        <v>0.5147415683279816</v>
       </c>
       <c r="C190">
-        <v>0.6747793197723282</v>
+        <v>0.675500706553442</v>
       </c>
       <c r="D190">
-        <v>0.6257408207262584</v>
+        <v>0.625822788818701</v>
       </c>
       <c r="E190">
-        <v>0.4553271303924059</v>
+        <v>0.4563012045541993</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -4542,16 +4542,16 @@
         <v>194</v>
       </c>
       <c r="B191">
-        <v>0.5366087569163752</v>
+        <v>0.517867544757795</v>
       </c>
       <c r="C191">
-        <v>0.5400000813745806</v>
+        <v>0.5253614659321036</v>
       </c>
       <c r="D191">
-        <v>0.5366087569163752</v>
+        <v>0.517867544757795</v>
       </c>
       <c r="E191">
-        <v>0.2916000878845536</v>
+        <v>0.2760046698863289</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -4559,16 +4559,16 @@
         <v>195</v>
       </c>
       <c r="B192">
-        <v>0.04302707252420216</v>
+        <v>0.04691302816246518</v>
       </c>
       <c r="C192">
-        <v>0.08242224794873147</v>
+        <v>0.08377354528513595</v>
       </c>
       <c r="D192">
-        <v>0.06552777343988458</v>
+        <v>0.06888169492650621</v>
       </c>
       <c r="E192">
-        <v>0.006793426956922169</v>
+        <v>0.007018006889640722</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -4644,16 +4644,16 @@
         <v>200</v>
       </c>
       <c r="B197">
-        <v>0.4422563550978273</v>
+        <v>0.4543731388645074</v>
       </c>
       <c r="C197">
-        <v>0.5824309960670567</v>
+        <v>0.5825160717613329</v>
       </c>
       <c r="D197">
-        <v>0.5211045820403631</v>
+        <v>0.527674799544215</v>
       </c>
       <c r="E197">
-        <v>0.3392258651796638</v>
+        <v>0.3393249738602544</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -4678,16 +4678,16 @@
         <v>202</v>
       </c>
       <c r="B199">
-        <v>0.3542423520977292</v>
+        <v>0.354309069232825</v>
       </c>
       <c r="C199">
-        <v>0.6702201097413079</v>
+        <v>0.6702896107596851</v>
       </c>
       <c r="D199">
-        <v>0.4684454702665165</v>
+        <v>0.4685180862783183</v>
       </c>
       <c r="E199">
-        <v>0.4491949955016508</v>
+        <v>0.4492881622923702</v>
       </c>
     </row>
     <row r="200" spans="1:5">
@@ -4712,16 +4712,16 @@
         <v>204</v>
       </c>
       <c r="B201">
-        <v>0.3774100401437214</v>
+        <v>0.3817970635207341</v>
       </c>
       <c r="C201">
-        <v>0.6771483019355148</v>
+        <v>0.6771324916338424</v>
       </c>
       <c r="D201">
-        <v>0.4800140030478471</v>
+        <v>0.4868262212926479</v>
       </c>
       <c r="E201">
-        <v>0.4585298228141512</v>
+        <v>0.4585084112262556</v>
       </c>
     </row>
     <row r="202" spans="1:5">
@@ -4729,16 +4729,16 @@
         <v>205</v>
       </c>
       <c r="B202">
-        <v>0.2299668212845014</v>
+        <v>0.2270252543935928</v>
       </c>
       <c r="C202">
-        <v>0.3331211687680439</v>
+        <v>0.3319284393845139</v>
       </c>
       <c r="D202">
-        <v>0.3141003606457448</v>
+        <v>0.3105454310880474</v>
       </c>
       <c r="E202">
-        <v>0.1109697130813876</v>
+        <v>0.1101764888722389</v>
       </c>
     </row>
     <row r="203" spans="1:5">
@@ -4746,16 +4746,16 @@
         <v>206</v>
       </c>
       <c r="B203">
-        <v>0.6636288510742434</v>
+        <v>0.6850619845483588</v>
       </c>
       <c r="C203">
-        <v>1.250548266361272</v>
+        <v>1.256665930215979</v>
       </c>
       <c r="D203">
-        <v>1.192010814737453</v>
+        <v>1.197844866702624</v>
       </c>
       <c r="E203">
-        <v>1.563870966499184</v>
+        <v>1.579209260165593</v>
       </c>
     </row>
     <row r="204" spans="1:5">
@@ -4763,16 +4763,16 @@
         <v>207</v>
       </c>
       <c r="B204">
-        <v>0.2720073406437508</v>
+        <v>0.2813260441005885</v>
       </c>
       <c r="C204">
-        <v>0.865641243069506</v>
+        <v>0.8919866067427858</v>
       </c>
       <c r="D204">
-        <v>0.7271737451664347</v>
+        <v>0.7537359771172792</v>
       </c>
       <c r="E204">
-        <v>0.7493347617029196</v>
+        <v>0.7956401066085093</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -4780,16 +4780,16 @@
         <v>208</v>
       </c>
       <c r="B205">
-        <v>0.3381162878718419</v>
+        <v>0.3682694247906502</v>
       </c>
       <c r="C205">
-        <v>0.4656077065095011</v>
+        <v>0.490309852296483</v>
       </c>
       <c r="D205">
-        <v>0.4402726896381634</v>
+        <v>0.464203551299002</v>
       </c>
       <c r="E205">
-        <v>0.2167905363610377</v>
+        <v>0.240403751258999</v>
       </c>
     </row>
     <row r="206" spans="1:5">
@@ -4797,16 +4797,16 @@
         <v>209</v>
       </c>
       <c r="B206">
-        <v>0.4348199296118083</v>
+        <v>0.431848350046943</v>
       </c>
       <c r="C206">
-        <v>0.7049524580910729</v>
+        <v>0.7050874089078224</v>
       </c>
       <c r="D206">
-        <v>0.5511732196639761</v>
+        <v>0.5449442067951729</v>
       </c>
       <c r="E206">
-        <v>0.4969579681686458</v>
+        <v>0.4971482542003468</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -4949,17 +4949,17 @@
       <c r="A215" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="B215">
-        <v>2.691251918718787</v>
-      </c>
-      <c r="C215">
-        <v>6.653489181362127</v>
-      </c>
-      <c r="D215">
-        <v>5.620729738993824</v>
-      </c>
-      <c r="E215">
-        <v>44.26891828650287</v>
+      <c r="B215" t="s">
+        <v>309</v>
+      </c>
+      <c r="C215" t="s">
+        <v>309</v>
+      </c>
+      <c r="D215" t="s">
+        <v>309</v>
+      </c>
+      <c r="E215" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="216" spans="1:5">
@@ -5035,16 +5035,16 @@
         <v>223</v>
       </c>
       <c r="B220">
-        <v>0.6541448590109735</v>
+        <v>0.6546045312585719</v>
       </c>
       <c r="C220">
-        <v>0.8783864813590151</v>
+        <v>0.8788923793035612</v>
       </c>
       <c r="D220">
-        <v>0.7204137188180217</v>
+        <v>0.7209220955102076</v>
       </c>
       <c r="E220">
-        <v>0.7715628106342713</v>
+        <v>0.7724518143978749</v>
       </c>
     </row>
     <row r="221" spans="1:5">
@@ -5188,16 +5188,16 @@
         <v>232</v>
       </c>
       <c r="B229">
-        <v>0.6636607920651172</v>
+        <v>0.6400073491773848</v>
       </c>
       <c r="C229">
-        <v>1.415273504786766</v>
+        <v>1.416171458422535</v>
       </c>
       <c r="D229">
-        <v>1.160586792805913</v>
+        <v>1.156040755653709</v>
       </c>
       <c r="E229">
-        <v>2.002999093351415</v>
+        <v>2.00554159965061</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -5205,16 +5205,16 @@
         <v>233</v>
       </c>
       <c r="B230">
-        <v>0.5305009644009041</v>
+        <v>0.6615317594669755</v>
       </c>
       <c r="C230">
-        <v>1.069410068995772</v>
+        <v>1.481794127734434</v>
       </c>
       <c r="D230">
-        <v>0.8851872053481238</v>
+        <v>1.147692270395905</v>
       </c>
       <c r="E230">
-        <v>1.143637895669542</v>
+        <v>2.195713836988252</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -5256,16 +5256,16 @@
         <v>236</v>
       </c>
       <c r="B233">
-        <v>0.4132584569004751</v>
+        <v>0.4147124726877563</v>
       </c>
       <c r="C233">
-        <v>0.6683420505163401</v>
+        <v>0.6704699075731598</v>
       </c>
       <c r="D233">
-        <v>0.5452728291645786</v>
+        <v>0.5444287890090957</v>
       </c>
       <c r="E233">
-        <v>0.4466810964883861</v>
+        <v>0.4495298969611614</v>
       </c>
     </row>
     <row r="234" spans="1:5">
@@ -5290,16 +5290,16 @@
         <v>238</v>
       </c>
       <c r="B235">
-        <v>0.4044238530327102</v>
+        <v>0.338737090717058</v>
       </c>
       <c r="C235">
-        <v>0.6576238432976542</v>
+        <v>0.5924390176407125</v>
       </c>
       <c r="D235">
-        <v>0.5265374031389407</v>
+        <v>0.4706481060637728</v>
       </c>
       <c r="E235">
-        <v>0.4324691192735776</v>
+        <v>0.3509839896230924</v>
       </c>
     </row>
     <row r="236" spans="1:5">
@@ -5324,16 +5324,16 @@
         <v>240</v>
       </c>
       <c r="B237">
-        <v>1.122223433871507</v>
+        <v>1.119783072995806</v>
       </c>
       <c r="C237">
-        <v>2.66784571967411</v>
+        <v>2.667912886861532</v>
       </c>
       <c r="D237">
-        <v>2.077419844667796</v>
+        <v>2.084350864327821</v>
       </c>
       <c r="E237">
-        <v>7.117400783983469</v>
+        <v>7.117759171881831</v>
       </c>
     </row>
     <row r="238" spans="1:5">
@@ -5341,16 +5341,16 @@
         <v>241</v>
       </c>
       <c r="B238">
-        <v>1.301367985539768</v>
+        <v>1.170409136832009</v>
       </c>
       <c r="C238">
-        <v>3.101432894385265</v>
+        <v>3.102044757762652</v>
       </c>
       <c r="D238">
-        <v>2.593663433800475</v>
+        <v>2.518040605413187</v>
       </c>
       <c r="E238">
-        <v>9.618885998374965</v>
+        <v>9.622681679162747</v>
       </c>
     </row>
     <row r="239" spans="1:5">
@@ -5375,16 +5375,16 @@
         <v>243</v>
       </c>
       <c r="B240">
-        <v>0.239779995656586</v>
+        <v>0.22588678651157</v>
       </c>
       <c r="C240">
-        <v>0.3665050536925023</v>
+        <v>0.377264594992349</v>
       </c>
       <c r="D240">
-        <v>0.2806401276258315</v>
+        <v>0.2478350435550793</v>
       </c>
       <c r="E240">
-        <v>0.134325954382144</v>
+        <v>0.1423285746347411</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -5443,16 +5443,16 @@
         <v>247</v>
       </c>
       <c r="B244">
-        <v>0.6430838391547367</v>
+        <v>0.6443347381830331</v>
       </c>
       <c r="C244">
-        <v>1.326744619732468</v>
+        <v>1.331398750509574</v>
       </c>
       <c r="D244">
-        <v>1.059816808925536</v>
+        <v>1.062536345324256</v>
       </c>
       <c r="E244">
-        <v>1.760251285989052</v>
+        <v>1.772622632858456</v>
       </c>
     </row>
     <row r="245" spans="1:5">
@@ -5460,16 +5460,16 @@
         <v>248</v>
       </c>
       <c r="B245">
-        <v>0.2695444680283904</v>
+        <v>0.2797860280492441</v>
       </c>
       <c r="C245">
-        <v>0.4827572310199679</v>
+        <v>0.4846615386535404</v>
       </c>
       <c r="D245">
-        <v>0.3869970451041957</v>
+        <v>0.3950544101162598</v>
       </c>
       <c r="E245">
-        <v>0.2330545441020666</v>
+        <v>0.2348968070500172</v>
       </c>
     </row>
     <row r="246" spans="1:5">
@@ -5477,16 +5477,16 @@
         <v>249</v>
       </c>
       <c r="B246">
-        <v>0.2957838582515955</v>
+        <v>0.2989509367180228</v>
       </c>
       <c r="C246">
-        <v>0.4594039256637149</v>
+        <v>0.5313605216075664</v>
       </c>
       <c r="D246">
-        <v>0.4000110957523126</v>
+        <v>0.3969826711253862</v>
       </c>
       <c r="E246">
-        <v>0.2110519669152321</v>
+        <v>0.282344003923065</v>
       </c>
     </row>
     <row r="247" spans="1:5">
@@ -5595,51 +5595,51 @@
       <c r="A253" s="1" t="s">
         <v>256</v>
       </c>
-      <c r="B253" t="s">
-        <v>309</v>
-      </c>
-      <c r="C253" t="s">
-        <v>309</v>
-      </c>
-      <c r="D253" t="s">
-        <v>309</v>
-      </c>
-      <c r="E253" t="s">
-        <v>309</v>
+      <c r="B253">
+        <v>1.847901766529964</v>
+      </c>
+      <c r="C253">
+        <v>4.206969902616522</v>
+      </c>
+      <c r="D253">
+        <v>3.527699938038989</v>
+      </c>
+      <c r="E253">
+        <v>17.69859576152126</v>
       </c>
     </row>
     <row r="254" spans="1:5">
       <c r="A254" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B254" t="s">
-        <v>309</v>
-      </c>
-      <c r="C254" t="s">
-        <v>309</v>
-      </c>
-      <c r="D254" t="s">
-        <v>309</v>
-      </c>
-      <c r="E254" t="s">
-        <v>309</v>
+      <c r="B254">
+        <v>0.943099052694421</v>
+      </c>
+      <c r="C254">
+        <v>2.421065142584239</v>
+      </c>
+      <c r="D254">
+        <v>1.997398223447031</v>
+      </c>
+      <c r="E254">
+        <v>5.861556424636441</v>
       </c>
     </row>
     <row r="255" spans="1:5">
       <c r="A255" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="B255">
-        <v>0.4979913503602915</v>
-      </c>
-      <c r="C255">
-        <v>0.9302740385373898</v>
-      </c>
-      <c r="D255">
-        <v>0.7654799244038171</v>
-      </c>
-      <c r="E255">
-        <v>0.865409786776665</v>
+      <c r="B255" t="s">
+        <v>309</v>
+      </c>
+      <c r="C255" t="s">
+        <v>309</v>
+      </c>
+      <c r="D255" t="s">
+        <v>309</v>
+      </c>
+      <c r="E255" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="256" spans="1:5">
@@ -5647,16 +5647,16 @@
         <v>259</v>
       </c>
       <c r="B256">
-        <v>0.2986338864781115</v>
+        <v>0.2987160853876935</v>
       </c>
       <c r="C256">
-        <v>0.6770198375847805</v>
+        <v>0.6771122867358185</v>
       </c>
       <c r="D256">
-        <v>0.458357049619408</v>
+        <v>0.4584518482273706</v>
       </c>
       <c r="E256">
-        <v>0.4583558604833225</v>
+        <v>0.4584810488486092</v>
       </c>
     </row>
     <row r="257" spans="1:5">
@@ -5732,16 +5732,16 @@
         <v>264</v>
       </c>
       <c r="B261">
-        <v>0.2488616520939965</v>
+        <v>0.2372409357851554</v>
       </c>
       <c r="C261">
-        <v>0.4174202458015729</v>
+        <v>0.4151739090789966</v>
       </c>
       <c r="D261">
-        <v>0.3318419027973536</v>
+        <v>0.3220384592416032</v>
       </c>
       <c r="E261">
-        <v>0.1742396616050456</v>
+        <v>0.1723693747799349</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -5834,16 +5834,16 @@
         <v>270</v>
       </c>
       <c r="B267">
-        <v>0.3377235641245172</v>
+        <v>0.356841870387845</v>
       </c>
       <c r="C267">
-        <v>0.526207763453406</v>
+        <v>0.5346972671727044</v>
       </c>
       <c r="D267">
-        <v>0.4591447985715182</v>
+        <v>0.4782790069557444</v>
       </c>
       <c r="E267">
-        <v>0.2768946103186358</v>
+        <v>0.2859011675219584</v>
       </c>
     </row>
     <row r="268" spans="1:5">
@@ -5851,16 +5851,16 @@
         <v>271</v>
       </c>
       <c r="B268">
-        <v>0.3568186762004948</v>
+        <v>0.366343111135018</v>
       </c>
       <c r="C268">
-        <v>0.5748677505120027</v>
+        <v>0.6516603423956933</v>
       </c>
       <c r="D268">
-        <v>0.4413935709855857</v>
+        <v>0.4483998193225938</v>
       </c>
       <c r="E268">
-        <v>0.3304729305787301</v>
+        <v>0.4246612018512722</v>
       </c>
     </row>
     <row r="269" spans="1:5">
@@ -5885,16 +5885,16 @@
         <v>273</v>
       </c>
       <c r="B270">
-        <v>0.427465147972562</v>
+        <v>0.4038481222007636</v>
       </c>
       <c r="C270">
-        <v>0.5429024404077392</v>
+        <v>0.6639234481123406</v>
       </c>
       <c r="D270">
-        <v>0.5005287750010116</v>
+        <v>0.489702463077172</v>
       </c>
       <c r="E270">
-        <v>0.2947430598006788</v>
+        <v>0.4407943449533798</v>
       </c>
     </row>
     <row r="271" spans="1:5">
@@ -5970,16 +5970,16 @@
         <v>278</v>
       </c>
       <c r="B275">
-        <v>0.7517366496852143</v>
+        <v>1.012127730012972</v>
       </c>
       <c r="C275">
-        <v>1.514999612805203</v>
+        <v>2.218502807536238</v>
       </c>
       <c r="D275">
-        <v>1.320475133835106</v>
+        <v>1.859351904188273</v>
       </c>
       <c r="E275">
-        <v>2.295223826799915</v>
+        <v>4.921754707046172</v>
       </c>
     </row>
     <row r="276" spans="1:5">
@@ -5987,16 +5987,16 @@
         <v>279</v>
       </c>
       <c r="B276">
-        <v>0.4199748094615064</v>
+        <v>0.4167929942469046</v>
       </c>
       <c r="C276">
-        <v>0.7027082191714312</v>
+        <v>0.7117039359144384</v>
       </c>
       <c r="D276">
-        <v>0.5953762474604262</v>
+        <v>0.6042125780971502</v>
       </c>
       <c r="E276">
-        <v>0.4937988412910843</v>
+        <v>0.506522492396103</v>
       </c>
     </row>
     <row r="277" spans="1:5">
@@ -6004,16 +6004,16 @@
         <v>280</v>
       </c>
       <c r="B277">
-        <v>0.2209026983737618</v>
+        <v>0.2323212356350655</v>
       </c>
       <c r="C277">
-        <v>0.4896859262918888</v>
+        <v>0.4885267643119551</v>
       </c>
       <c r="D277">
-        <v>0.3306289147645877</v>
+        <v>0.3422972784598408</v>
       </c>
       <c r="E277">
-        <v>0.2397923064083451</v>
+        <v>0.2386583994491086</v>
       </c>
     </row>
     <row r="278" spans="1:5">
@@ -6055,16 +6055,16 @@
         <v>283</v>
       </c>
       <c r="B280">
-        <v>0.3443057757722173</v>
+        <v>0.4559632453887983</v>
       </c>
       <c r="C280">
-        <v>0.5139208504711065</v>
+        <v>0.7408190345064148</v>
       </c>
       <c r="D280">
-        <v>0.4442644792455555</v>
+        <v>0.5682576978759625</v>
       </c>
       <c r="E280">
-        <v>0.2641146405489453</v>
+        <v>0.5488128418870166</v>
       </c>
     </row>
     <row r="281" spans="1:5">
@@ -6072,16 +6072,16 @@
         <v>284</v>
       </c>
       <c r="B281">
-        <v>0.3609006479437549</v>
+        <v>0.3953213598971483</v>
       </c>
       <c r="C281">
-        <v>0.7027422837819506</v>
+        <v>0.728719261443752</v>
       </c>
       <c r="D281">
-        <v>0.5166305694158154</v>
+        <v>0.567269928455555</v>
       </c>
       <c r="E281">
-        <v>0.4938467174150715</v>
+        <v>0.5310317619991274</v>
       </c>
     </row>
     <row r="282" spans="1:5">
@@ -6089,16 +6089,16 @@
         <v>285</v>
       </c>
       <c r="B282">
-        <v>0.2755854682114368</v>
+        <v>0.3011209720807008</v>
       </c>
       <c r="C282">
-        <v>0.5486141495397101</v>
+        <v>0.5438323979128884</v>
       </c>
       <c r="D282">
-        <v>0.3901489660233114</v>
+        <v>0.411050394874993</v>
       </c>
       <c r="E282">
-        <v>0.3009774850751794</v>
+        <v>0.2957536770196821</v>
       </c>
     </row>
     <row r="283" spans="1:5">
@@ -6106,16 +6106,16 @@
         <v>286</v>
       </c>
       <c r="B283">
-        <v>0.03260134632405208</v>
+        <v>0.04057552673830871</v>
       </c>
       <c r="C283">
-        <v>1.908059709919542</v>
+        <v>2.25326691270073</v>
       </c>
       <c r="D283">
-        <v>1.401568455853855</v>
+        <v>1.753145101197639</v>
       </c>
       <c r="E283">
-        <v>3.640691856618246</v>
+        <v>5.077211779871879</v>
       </c>
     </row>
     <row r="284" spans="1:5">
@@ -6123,16 +6123,16 @@
         <v>287</v>
       </c>
       <c r="B284">
-        <v>0.7643049073155028</v>
+        <v>0.4403470546450587</v>
       </c>
       <c r="C284">
-        <v>1.225708385256284</v>
+        <v>0.7935493860305144</v>
       </c>
       <c r="D284">
-        <v>0.986216419621204</v>
+        <v>0.6538193846203092</v>
       </c>
       <c r="E284">
-        <v>1.502361045687567</v>
+        <v>0.6297206280694064</v>
       </c>
     </row>
     <row r="285" spans="1:5">
@@ -6140,16 +6140,16 @@
         <v>288</v>
       </c>
       <c r="B285">
-        <v>0.5678790023479904</v>
+        <v>0.4649488761211918</v>
       </c>
       <c r="C285">
-        <v>0.7966269224191548</v>
+        <v>0.7351609215819723</v>
       </c>
       <c r="D285">
-        <v>0.6377084498162536</v>
+        <v>0.5568012811605045</v>
       </c>
       <c r="E285">
-        <v>0.634614453523014</v>
+        <v>0.5404615806212548</v>
       </c>
     </row>
     <row r="286" spans="1:5">
@@ -6157,16 +6157,16 @@
         <v>289</v>
       </c>
       <c r="B286">
-        <v>0.3236588514293864</v>
+        <v>0.3096570741416385</v>
       </c>
       <c r="C286">
-        <v>0.5061657064880014</v>
+        <v>0.579074492212317</v>
       </c>
       <c r="D286">
-        <v>0.4551911377758415</v>
+        <v>0.4616490810363906</v>
       </c>
       <c r="E286">
-        <v>0.2562037224244976</v>
+        <v>0.3353272675309527</v>
       </c>
     </row>
     <row r="287" spans="1:5">
@@ -6191,16 +6191,16 @@
         <v>291</v>
       </c>
       <c r="B288">
-        <v>0.08814742572482767</v>
+        <v>0.08261384965669537</v>
       </c>
       <c r="C288">
-        <v>0.3558483318097517</v>
+        <v>0.3505267337930467</v>
       </c>
       <c r="D288">
-        <v>0.2632085948214236</v>
+        <v>0.2446767732362185</v>
       </c>
       <c r="E288">
-        <v>0.1266280352517831</v>
+        <v>0.1228689911036214</v>
       </c>
     </row>
     <row r="289" spans="1:5">
@@ -6208,16 +6208,16 @@
         <v>292</v>
       </c>
       <c r="B289">
-        <v>0.4648656027374697</v>
+        <v>0.5072163124376119</v>
       </c>
       <c r="C289">
-        <v>0.8275623328992054</v>
+        <v>0.9151044148818931</v>
       </c>
       <c r="D289">
-        <v>0.7177890282533482</v>
+        <v>0.772049689206718</v>
       </c>
       <c r="E289">
-        <v>0.6848594148335753</v>
+        <v>0.8374160901363319</v>
       </c>
     </row>
     <row r="290" spans="1:5">
@@ -6225,16 +6225,16 @@
         <v>293</v>
       </c>
       <c r="B290">
-        <v>0.2953475001595469</v>
+        <v>0.3159413762861042</v>
       </c>
       <c r="C290">
-        <v>0.592708992349585</v>
+        <v>0.5924856852129647</v>
       </c>
       <c r="D290">
-        <v>0.4161926673382532</v>
+        <v>0.4327241039814879</v>
       </c>
       <c r="E290">
-        <v>0.3513039496120604</v>
+        <v>0.3510392871822763</v>
       </c>
     </row>
     <row r="291" spans="1:5">
@@ -6259,16 +6259,16 @@
         <v>295</v>
       </c>
       <c r="B292">
-        <v>0.856976496308628</v>
+        <v>0.8041194754295797</v>
       </c>
       <c r="C292">
-        <v>1.116821319520697</v>
+        <v>1.056051084389874</v>
       </c>
       <c r="D292">
-        <v>0.964363718864836</v>
+        <v>0.8929986523985423</v>
       </c>
       <c r="E292">
-        <v>1.247289859735952</v>
+        <v>1.115243892841029</v>
       </c>
     </row>
     <row r="293" spans="1:5">
@@ -6310,16 +6310,16 @@
         <v>298</v>
       </c>
       <c r="B295">
-        <v>0.4885471685577798</v>
+        <v>0.4839785394034826</v>
       </c>
       <c r="C295">
-        <v>0.7394537997407816</v>
+        <v>0.7322927666818866</v>
       </c>
       <c r="D295">
-        <v>0.6883779266685522</v>
+        <v>0.6976449120474562</v>
       </c>
       <c r="E295">
-        <v>0.54679192195108</v>
+        <v>0.536252696134612</v>
       </c>
     </row>
     <row r="296" spans="1:5">
@@ -6327,16 +6327,16 @@
         <v>299</v>
       </c>
       <c r="B296">
-        <v>0.3729948090833025</v>
+        <v>0.3734568368740922</v>
       </c>
       <c r="C296">
-        <v>0.6445662341691769</v>
+        <v>0.6437817175565815</v>
       </c>
       <c r="D296">
-        <v>0.5163738933911457</v>
+        <v>0.5093849003613893</v>
       </c>
       <c r="E296">
-        <v>0.4154656302310342</v>
+        <v>0.4144548998601021</v>
       </c>
     </row>
     <row r="297" spans="1:5">
@@ -6344,16 +6344,16 @@
         <v>300</v>
       </c>
       <c r="B297">
-        <v>0.2670472026357783</v>
+        <v>0.3296129858595937</v>
       </c>
       <c r="C297">
-        <v>0.4434383747642636</v>
+        <v>0.635126615704628</v>
       </c>
       <c r="D297">
-        <v>0.3630258893849641</v>
+        <v>0.4275774474262181</v>
       </c>
       <c r="E297">
-        <v>0.1966375922135715</v>
+        <v>0.4033858179764142</v>
       </c>
     </row>
     <row r="298" spans="1:5">
@@ -6361,16 +6361,16 @@
         <v>301</v>
       </c>
       <c r="B298">
-        <v>0.315948283213447</v>
+        <v>0.3418105859081604</v>
       </c>
       <c r="C298">
-        <v>0.4491388841734102</v>
+        <v>0.453774831740368</v>
       </c>
       <c r="D298">
-        <v>0.4103388918110319</v>
+        <v>0.4309412298432656</v>
       </c>
       <c r="E298">
-        <v>0.201725737276536</v>
+        <v>0.2059115979209993</v>
       </c>
     </row>
     <row r="299" spans="1:5">
@@ -6378,16 +6378,16 @@
         <v>302</v>
       </c>
       <c r="B299">
-        <v>0.3533408825505001</v>
+        <v>0.2985221606993849</v>
       </c>
       <c r="C299">
-        <v>0.5748121950417222</v>
+        <v>0.512826995332812</v>
       </c>
       <c r="D299">
-        <v>0.4785190135778719</v>
+        <v>0.3989242486639109</v>
       </c>
       <c r="E299">
-        <v>0.3304090595686828</v>
+        <v>0.2629915271420799</v>
       </c>
     </row>
     <row r="300" spans="1:5">
@@ -6395,16 +6395,16 @@
         <v>303</v>
       </c>
       <c r="B300">
-        <v>0.3153749232996019</v>
+        <v>0.3157810489896443</v>
       </c>
       <c r="C300">
-        <v>0.5921180872487012</v>
+        <v>0.5913873123135934</v>
       </c>
       <c r="D300">
-        <v>0.4499092342780673</v>
+        <v>0.4503317776032997</v>
       </c>
       <c r="E300">
-        <v>0.3506038292470605</v>
+        <v>0.3497389531654956</v>
       </c>
     </row>
     <row r="301" spans="1:5">
@@ -6446,16 +6446,16 @@
         <v>306</v>
       </c>
       <c r="B303">
-        <v>0.4508015852393508</v>
+        <v>0.4539341939744569</v>
       </c>
       <c r="C303">
-        <v>0.9016031704787015</v>
+        <v>0.9078683879489138</v>
       </c>
       <c r="D303">
-        <v>0.9016031704787015</v>
+        <v>0.9078683879489138</v>
       </c>
       <c r="E303">
-        <v>0.8128882770172465</v>
+        <v>0.8242250098369595</v>
       </c>
     </row>
     <row r="304" spans="1:5">
@@ -6480,16 +6480,16 @@
         <v>308</v>
       </c>
       <c r="B305">
-        <v>0.6004553179288166</v>
+        <v>0.6009216450710479</v>
       </c>
       <c r="C305">
-        <v>0.9388860798712521</v>
+        <v>0.9387982097290376</v>
       </c>
       <c r="D305">
-        <v>0.8573679400186333</v>
+        <v>0.8575703055954209</v>
       </c>
       <c r="E305">
-        <v>0.8815070709760071</v>
+        <v>0.881342078590446</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ejecucion actualizada r_q varios escenarios
</commit_message>
<xml_diff>
--- a/src/datos/metricas_holt_winters.xlsx
+++ b/src/datos/metricas_holt_winters.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="590" uniqueCount="311">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="311">
   <si>
     <t>MAPE</t>
   </si>
@@ -1347,7 +1347,7 @@
         <v>310</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -1372,19 +1372,19 @@
         <v>8</v>
       </c>
       <c r="B4">
-        <v>0.4785197544389728</v>
+        <v>0.3148538133851255</v>
       </c>
       <c r="C4">
-        <v>0.7549326147219918</v>
+        <v>0.4862673192375435</v>
       </c>
       <c r="D4">
-        <v>0.5699235432927258</v>
+        <v>0.4342931644885453</v>
       </c>
       <c r="E4">
-        <v>0.5699232527709833</v>
+        <v>0.236455905758467</v>
       </c>
       <c r="F4">
-        <v>-33.33600052953668</v>
+        <v>9.307478550342296</v>
       </c>
     </row>
     <row r="5" spans="1:6">
@@ -1409,19 +1409,19 @@
         <v>10</v>
       </c>
       <c r="B6">
-        <v>0.4842677233844159</v>
+        <v>0.3640163802844195</v>
       </c>
       <c r="C6">
-        <v>0.7361164912496631</v>
+        <v>0.6126708994008504</v>
       </c>
       <c r="D6">
-        <v>0.5792221627234778</v>
+        <v>0.5035046148619263</v>
       </c>
       <c r="E6">
-        <v>0.5418674886897152</v>
+        <v>0.3753656309726469</v>
       </c>
       <c r="F6">
-        <v>-21.3112310254769</v>
+        <v>13.06278614043642</v>
       </c>
     </row>
     <row r="7" spans="1:6">
@@ -1441,7 +1441,7 @@
         <v>310</v>
       </c>
       <c r="F7">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="8" spans="1:6">
@@ -1449,19 +1449,19 @@
         <v>12</v>
       </c>
       <c r="B8">
-        <v>0.2742789812315319</v>
+        <v>0.2702126261711809</v>
       </c>
       <c r="C8">
-        <v>1.653201196005105</v>
+        <v>1.600240598130502</v>
       </c>
       <c r="D8">
-        <v>1.158103701997333</v>
+        <v>1.170869767809569</v>
       </c>
       <c r="E8">
-        <v>2.733074194472709</v>
+        <v>2.560769971905068</v>
       </c>
       <c r="F8">
-        <v>-2.610705718425087</v>
+        <v>-2.075550712450908</v>
       </c>
     </row>
     <row r="9" spans="1:6">
@@ -1481,7 +1481,7 @@
         <v>310</v>
       </c>
       <c r="F9">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="10" spans="1:6">
@@ -1501,7 +1501,7 @@
         <v>310</v>
       </c>
       <c r="F10">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1509,19 +1509,19 @@
         <v>15</v>
       </c>
       <c r="B11">
-        <v>0.2479499280673633</v>
+        <v>0.2543455685148411</v>
       </c>
       <c r="C11">
-        <v>0.4908884338090687</v>
+        <v>0.4906085445383461</v>
       </c>
       <c r="D11">
-        <v>0.3679259083736022</v>
+        <v>0.3695116294941737</v>
       </c>
       <c r="E11">
-        <v>0.2409714544475204</v>
+        <v>0.2406967439740344</v>
       </c>
       <c r="F11">
-        <v>-0.7490597267154374</v>
+        <v>-0.6716420665555399</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1529,19 +1529,19 @@
         <v>16</v>
       </c>
       <c r="B12">
-        <v>0.2152136891183062</v>
+        <v>0.1940544555164662</v>
       </c>
       <c r="C12">
-        <v>0.4643190849706741</v>
+        <v>0.4712396563385006</v>
       </c>
       <c r="D12">
-        <v>0.4304273782366124</v>
+        <v>0.3881089110329323</v>
       </c>
       <c r="E12">
-        <v>0.2155922126680041</v>
+        <v>0.2220668137060281</v>
       </c>
       <c r="F12">
-        <v>-0.8091458722835078</v>
+        <v>-1.37734233689049</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1549,19 +1549,19 @@
         <v>17</v>
       </c>
       <c r="B13">
-        <v>0.4973142522638217</v>
+        <v>0.4962002659303797</v>
       </c>
       <c r="C13">
-        <v>0.703858271966591</v>
+        <v>0.7026007552634912</v>
       </c>
       <c r="D13">
-        <v>0.6681950648773829</v>
+        <v>0.671004708060645</v>
       </c>
       <c r="E13">
-        <v>0.4954164670157957</v>
+        <v>0.4936478212968283</v>
       </c>
       <c r="F13">
-        <v>0.06881906070201795</v>
+        <v>0.1261379843755113</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1569,19 +1569,19 @@
         <v>18</v>
       </c>
       <c r="B14">
-        <v>0.92954526580872</v>
+        <v>0.9986311598465477</v>
       </c>
       <c r="C14">
-        <v>2.362115868946816</v>
+        <v>2.386764893631082</v>
       </c>
       <c r="D14">
-        <v>1.890812397032165</v>
+        <v>1.960041068635253</v>
       </c>
       <c r="E14">
-        <v>5.579591378330373</v>
+        <v>5.696646657469792</v>
       </c>
       <c r="F14">
-        <v>13.9196193704886</v>
+        <v>5.039094924643603</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1601,7 +1601,7 @@
         <v>310</v>
       </c>
       <c r="F15">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1672,7 +1672,7 @@
         <v>310</v>
       </c>
       <c r="F19">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="20" spans="1:6">
@@ -1680,19 +1680,19 @@
         <v>24</v>
       </c>
       <c r="B20">
-        <v>0.2742904583252281</v>
+        <v>0.2576611117421613</v>
       </c>
       <c r="C20">
-        <v>0.6240427714932152</v>
+        <v>0.5939996345868173</v>
       </c>
       <c r="D20">
-        <v>0.4176941020477056</v>
+        <v>0.4017653267140427</v>
       </c>
       <c r="E20">
-        <v>0.3894293806529332</v>
+        <v>0.3528355658892724</v>
       </c>
       <c r="F20">
-        <v>58.09476870122729</v>
+        <v>69.79153309487931</v>
       </c>
     </row>
     <row r="21" spans="1:6">
@@ -1734,39 +1734,39 @@
         <v>27</v>
       </c>
       <c r="B23">
-        <v>0.1218552397721261</v>
+        <v>0.1239113776277215</v>
       </c>
       <c r="C23">
-        <v>2.049363897780487</v>
+        <v>2.070806347774355</v>
       </c>
       <c r="D23">
-        <v>1.781907636246735</v>
+        <v>1.809838279343709</v>
       </c>
       <c r="E23">
-        <v>4.199892385526029</v>
+        <v>4.288238929982562</v>
       </c>
       <c r="F23">
-        <v>0.4968055566449042</v>
+        <v>0.5207624390252656</v>
       </c>
     </row>
     <row r="24" spans="1:6">
       <c r="A24" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B24">
-        <v>0.6252739392370442</v>
-      </c>
-      <c r="C24">
-        <v>1.283957647020595</v>
-      </c>
-      <c r="D24">
-        <v>1.044723787105006</v>
-      </c>
-      <c r="E24">
-        <v>1.648547239342663</v>
+      <c r="B24" t="s">
+        <v>310</v>
+      </c>
+      <c r="C24" t="s">
+        <v>310</v>
+      </c>
+      <c r="D24" t="s">
+        <v>310</v>
+      </c>
+      <c r="E24" t="s">
+        <v>310</v>
       </c>
       <c r="F24">
-        <v>-14.36373071749691</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="25" spans="1:6">
@@ -1774,19 +1774,19 @@
         <v>29</v>
       </c>
       <c r="B25">
-        <v>0.1346119527790017</v>
+        <v>0.1320954441718596</v>
       </c>
       <c r="C25">
-        <v>0.4735463645298876</v>
+        <v>0.4680118333528058</v>
       </c>
       <c r="D25">
-        <v>0.2528801812939429</v>
+        <v>0.248987919441852</v>
       </c>
       <c r="E25">
-        <v>0.2242461593594732</v>
+        <v>0.2190350761582545</v>
       </c>
       <c r="F25">
-        <v>3.830923447956268</v>
+        <v>3.613361462721508</v>
       </c>
     </row>
     <row r="26" spans="1:6">
@@ -1806,7 +1806,7 @@
         <v>310</v>
       </c>
       <c r="F26">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="27" spans="1:6">
@@ -1826,7 +1826,7 @@
         <v>310</v>
       </c>
       <c r="F27">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="28" spans="1:6">
@@ -1834,19 +1834,19 @@
         <v>32</v>
       </c>
       <c r="B28">
-        <v>0.3437598528941487</v>
+        <v>0.3436801659851091</v>
       </c>
       <c r="C28">
-        <v>0.4330265709682471</v>
+        <v>0.4330897669944608</v>
       </c>
       <c r="D28">
-        <v>0.3750073754666303</v>
+        <v>0.3748691125198659</v>
       </c>
       <c r="E28">
-        <v>0.1875120111645184</v>
+        <v>0.1875667462753164</v>
       </c>
       <c r="F28">
-        <v>-9.888183625814905E-05</v>
+        <v>-0.004213981469932822</v>
       </c>
     </row>
     <row r="29" spans="1:6">
@@ -1866,7 +1866,7 @@
         <v>310</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="30" spans="1:6">
@@ -1886,7 +1886,7 @@
         <v>310</v>
       </c>
       <c r="F30">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="31" spans="1:6">
@@ -1911,19 +1911,19 @@
         <v>36</v>
       </c>
       <c r="B32">
-        <v>0.350190397037375</v>
+        <v>0.3500430347916481</v>
       </c>
       <c r="C32">
-        <v>0.6611638575389572</v>
+        <v>0.6612235821119842</v>
       </c>
       <c r="D32">
-        <v>0.473070156715047</v>
+        <v>0.4729584689169352</v>
       </c>
       <c r="E32">
-        <v>0.4371376465157945</v>
+        <v>0.4372166255410039</v>
       </c>
       <c r="F32">
-        <v>1.058539682527039</v>
+        <v>1.138790352501047</v>
       </c>
     </row>
     <row r="33" spans="1:6">
@@ -1931,19 +1931,19 @@
         <v>37</v>
       </c>
       <c r="B33">
-        <v>0.3121813045966073</v>
+        <v>0.3136320439497087</v>
       </c>
       <c r="C33">
-        <v>0.6008565807941408</v>
+        <v>0.6016242398722035</v>
       </c>
       <c r="D33">
-        <v>0.4118525270682897</v>
+        <v>0.4136078176725643</v>
       </c>
       <c r="E33">
-        <v>0.3610286306836259</v>
+        <v>0.3619517260018066</v>
       </c>
       <c r="F33">
-        <v>32.02557575601035</v>
+        <v>32.672198236756</v>
       </c>
     </row>
     <row r="34" spans="1:6">
@@ -1963,27 +1963,27 @@
         <v>310</v>
       </c>
       <c r="F34">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="35" spans="1:6">
       <c r="A35" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="B35">
-        <v>0.4943542603197967</v>
-      </c>
-      <c r="C35">
-        <v>1.058295163498508</v>
-      </c>
-      <c r="D35">
-        <v>0.9002780937351358</v>
-      </c>
-      <c r="E35">
-        <v>1.119988653084334</v>
+      <c r="B35" t="s">
+        <v>310</v>
+      </c>
+      <c r="C35" t="s">
+        <v>310</v>
+      </c>
+      <c r="D35" t="s">
+        <v>310</v>
+      </c>
+      <c r="E35" t="s">
+        <v>310</v>
       </c>
       <c r="F35">
-        <v>36.50174097189687</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="36" spans="1:6">
@@ -1991,19 +1991,19 @@
         <v>40</v>
       </c>
       <c r="B36">
-        <v>0.5078464688119194</v>
+        <v>0.4961241288461042</v>
       </c>
       <c r="C36">
-        <v>0.8973560188283011</v>
+        <v>0.9144598118568728</v>
       </c>
       <c r="D36">
-        <v>0.7690253568404575</v>
+        <v>0.7771087635266259</v>
       </c>
       <c r="E36">
-        <v>0.8052478245273782</v>
+        <v>0.8362367475013072</v>
       </c>
       <c r="F36">
-        <v>-6.996766110717362</v>
+        <v>12.57404380404273</v>
       </c>
     </row>
     <row r="37" spans="1:6">
@@ -2011,19 +2011,19 @@
         <v>41</v>
       </c>
       <c r="B37">
-        <v>0.4812766691317129</v>
+        <v>0.5587640823326054</v>
       </c>
       <c r="C37">
-        <v>1.083179294813717</v>
+        <v>1.162445445364535</v>
       </c>
       <c r="D37">
-        <v>0.8960473044056296</v>
+        <v>0.9690740690889453</v>
       </c>
       <c r="E37">
-        <v>1.173277384713141</v>
+        <v>1.351279413448753</v>
       </c>
       <c r="F37">
-        <v>88.0655986779858</v>
+        <v>20.29256692835275</v>
       </c>
     </row>
     <row r="38" spans="1:6">
@@ -2082,19 +2082,19 @@
         <v>45</v>
       </c>
       <c r="B41">
-        <v>0.346475075612799</v>
+        <v>0.395896570936929</v>
       </c>
       <c r="C41">
-        <v>0.5374407837963875</v>
+        <v>0.5847283181745248</v>
       </c>
       <c r="D41">
-        <v>0.4767901057640782</v>
+        <v>0.5000111684757351</v>
       </c>
       <c r="E41">
-        <v>0.2888425960876754</v>
+        <v>0.3419072060752082</v>
       </c>
       <c r="F41">
-        <v>8.580801732072791</v>
+        <v>-16.46492616269211</v>
       </c>
     </row>
     <row r="42" spans="1:6">
@@ -2238,19 +2238,19 @@
         <v>54</v>
       </c>
       <c r="B50">
-        <v>0.3786523262858459</v>
+        <v>0.4731135362636026</v>
       </c>
       <c r="C50">
-        <v>0.820202901680237</v>
+        <v>1.020614382255452</v>
       </c>
       <c r="D50">
-        <v>0.666717698527035</v>
+        <v>0.7677676495059794</v>
       </c>
       <c r="E50">
-        <v>0.6727327999246806</v>
+        <v>1.041653717266678</v>
       </c>
       <c r="F50">
-        <v>115.8801348881968</v>
+        <v>45.63924081755496</v>
       </c>
     </row>
     <row r="51" spans="1:6">
@@ -2258,19 +2258,19 @@
         <v>55</v>
       </c>
       <c r="B51">
-        <v>0.3079693366640604</v>
+        <v>0.3405987478793847</v>
       </c>
       <c r="C51">
-        <v>0.6369961817261671</v>
+        <v>0.4950945878915454</v>
       </c>
       <c r="D51">
-        <v>0.4505273714910333</v>
+        <v>0.4354719288921718</v>
       </c>
       <c r="E51">
-        <v>0.4057641355337161</v>
+        <v>0.2451186509594991</v>
       </c>
       <c r="F51">
-        <v>38.10204834265534</v>
+        <v>-8.484192147371221</v>
       </c>
     </row>
     <row r="52" spans="1:6">
@@ -2329,19 +2329,19 @@
         <v>59</v>
       </c>
       <c r="B55">
-        <v>0.2728131712898962</v>
+        <v>0.2810152711713801</v>
       </c>
       <c r="C55">
-        <v>0.5962267099981418</v>
+        <v>0.4288356833243861</v>
       </c>
       <c r="D55">
-        <v>0.3911057010656378</v>
+        <v>0.3722335916842375</v>
       </c>
       <c r="E55">
-        <v>0.3554862897152082</v>
+        <v>0.1839000432922931</v>
       </c>
       <c r="F55">
-        <v>40.3266870744098</v>
+        <v>-1.740055873937763</v>
       </c>
     </row>
     <row r="56" spans="1:6">
@@ -2378,7 +2378,7 @@
         <v>310</v>
       </c>
       <c r="F57">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="58" spans="1:6">
@@ -2398,7 +2398,7 @@
         <v>310</v>
       </c>
       <c r="F58">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="59" spans="1:6">
@@ -2423,19 +2423,19 @@
         <v>64</v>
       </c>
       <c r="B60">
-        <v>0.2805271758071332</v>
+        <v>0.2825009315395608</v>
       </c>
       <c r="C60">
-        <v>0.5235812168825181</v>
+        <v>0.5273740552319763</v>
       </c>
       <c r="D60">
-        <v>0.3879917707763333</v>
+        <v>0.3932168827660884</v>
       </c>
       <c r="E60">
-        <v>0.2741372906721785</v>
+        <v>0.2781233941318196</v>
       </c>
       <c r="F60">
-        <v>7.407407549780036</v>
+        <v>8.959734012984644</v>
       </c>
     </row>
     <row r="61" spans="1:6">
@@ -2443,19 +2443,19 @@
         <v>65</v>
       </c>
       <c r="B61">
-        <v>0.3665825999630865</v>
+        <v>0.3617912147026882</v>
       </c>
       <c r="C61">
-        <v>0.5315375825263128</v>
+        <v>0.6743280718580542</v>
       </c>
       <c r="D61">
-        <v>0.4799963068238096</v>
+        <v>0.4816526715954902</v>
       </c>
       <c r="E61">
-        <v>0.2825322016379168</v>
+        <v>0.4547183484958011</v>
       </c>
       <c r="F61">
-        <v>-4.664672864243195</v>
+        <v>-3.689886612562021</v>
       </c>
     </row>
     <row r="62" spans="1:6">
@@ -2463,19 +2463,19 @@
         <v>66</v>
       </c>
       <c r="B62">
-        <v>0.2099258827524449</v>
+        <v>0.3619509764589753</v>
       </c>
       <c r="C62">
-        <v>0.4885537687981014</v>
+        <v>0.5501198617053455</v>
       </c>
       <c r="D62">
-        <v>0.3275930622877272</v>
+        <v>0.4488442853540675</v>
       </c>
       <c r="E62">
-        <v>0.2386847850068287</v>
+        <v>0.3026318622427085</v>
       </c>
       <c r="F62">
-        <v>23.58439877245576</v>
+        <v>-7.296401706232898</v>
       </c>
     </row>
     <row r="63" spans="1:6">
@@ -2500,19 +2500,19 @@
         <v>68</v>
       </c>
       <c r="B64">
-        <v>0.4269978170481862</v>
+        <v>0.4241868725429141</v>
       </c>
       <c r="C64">
-        <v>0.7052748069107827</v>
+        <v>0.6666674898751805</v>
       </c>
       <c r="D64">
-        <v>0.5343134595692526</v>
+        <v>0.53426740379045</v>
       </c>
       <c r="E64">
-        <v>0.4974125532630419</v>
+        <v>0.444445542056474</v>
       </c>
       <c r="F64">
-        <v>-24.21967324949678</v>
+        <v>-8.877128578152053</v>
       </c>
     </row>
     <row r="65" spans="1:6">
@@ -2588,19 +2588,19 @@
         <v>73</v>
       </c>
       <c r="B69">
-        <v>0.4024689269396064</v>
+        <v>0.3382537911238662</v>
       </c>
       <c r="C69">
-        <v>0.7084162246641942</v>
+        <v>0.4808996486264909</v>
       </c>
       <c r="D69">
-        <v>0.5092506282879687</v>
+        <v>0.4549239627717098</v>
       </c>
       <c r="E69">
-        <v>0.50185354736747</v>
+        <v>0.2312644720490825</v>
       </c>
       <c r="F69">
-        <v>-17.00244929174152</v>
+        <v>2.429267590819456</v>
       </c>
     </row>
     <row r="70" spans="1:6">
@@ -2659,19 +2659,19 @@
         <v>77</v>
       </c>
       <c r="B73">
-        <v>0.2421687401130112</v>
+        <v>0.2443624348446876</v>
       </c>
       <c r="C73">
-        <v>0.5666187797404549</v>
+        <v>0.524644137459496</v>
       </c>
       <c r="D73">
-        <v>0.3956829827225543</v>
+        <v>0.3854809468793123</v>
       </c>
       <c r="E73">
-        <v>0.3210568415545622</v>
+        <v>0.2752514709706186</v>
       </c>
       <c r="F73">
-        <v>108.7614167909338</v>
+        <v>80.15815939732623</v>
       </c>
     </row>
     <row r="74" spans="1:6">
@@ -2679,19 +2679,19 @@
         <v>78</v>
       </c>
       <c r="B74">
-        <v>0.7213099399472817</v>
+        <v>0.7278822437105076</v>
       </c>
       <c r="C74">
-        <v>1.248816626346622</v>
+        <v>1.242303151702643</v>
       </c>
       <c r="D74">
-        <v>1.041230487736015</v>
+        <v>1.03798643057509</v>
       </c>
       <c r="E74">
-        <v>1.559542966239758</v>
+        <v>1.543317120730319</v>
       </c>
       <c r="F74">
-        <v>2.506454042107869</v>
+        <v>1.800713977335255</v>
       </c>
     </row>
     <row r="75" spans="1:6">
@@ -2716,19 +2716,19 @@
         <v>80</v>
       </c>
       <c r="B76">
-        <v>0.5386093494891809</v>
+        <v>0.512463498814238</v>
       </c>
       <c r="C76">
-        <v>0.771125856334709</v>
+        <v>0.5874047807749982</v>
       </c>
       <c r="D76">
-        <v>0.6001724274718858</v>
+        <v>0.568639150236622</v>
       </c>
       <c r="E76">
-        <v>0.5946350863079382</v>
+        <v>0.3450443764773238</v>
       </c>
       <c r="F76">
-        <v>-57.2488498417727</v>
+        <v>-55.04057457310321</v>
       </c>
     </row>
     <row r="77" spans="1:6">
@@ -2770,19 +2770,19 @@
         <v>83</v>
       </c>
       <c r="B79">
-        <v>0.3746648148250004</v>
+        <v>0.3066547200232617</v>
       </c>
       <c r="C79">
-        <v>0.5128566683136849</v>
+        <v>0.5025128827172471</v>
       </c>
       <c r="D79">
-        <v>0.4794341518489014</v>
+        <v>0.4397155519470099</v>
       </c>
       <c r="E79">
-        <v>0.2630219622338131</v>
+        <v>0.2525191972967978</v>
       </c>
       <c r="F79">
-        <v>-12.46328311934621</v>
+        <v>20.83221700594803</v>
       </c>
     </row>
     <row r="80" spans="1:6">
@@ -2824,19 +2824,19 @@
         <v>86</v>
       </c>
       <c r="B82">
-        <v>0.3305621246278342</v>
+        <v>0.3351790835448378</v>
       </c>
       <c r="C82">
-        <v>0.5192314270491738</v>
+        <v>0.5203213853177948</v>
       </c>
       <c r="D82">
-        <v>0.4609956280402415</v>
+        <v>0.4603433590890936</v>
       </c>
       <c r="E82">
-        <v>0.2696012748355215</v>
+        <v>0.2707343440190291</v>
       </c>
       <c r="F82">
-        <v>2.503341152028515</v>
+        <v>1.663890883939996</v>
       </c>
     </row>
     <row r="83" spans="1:6">
@@ -2844,19 +2844,19 @@
         <v>87</v>
       </c>
       <c r="B83">
-        <v>0.3964865959018274</v>
+        <v>0.3888477535631482</v>
       </c>
       <c r="C83">
-        <v>0.7083676044036145</v>
+        <v>0.709697051141873</v>
       </c>
       <c r="D83">
-        <v>0.519281881305712</v>
+        <v>0.5143598422736415</v>
       </c>
       <c r="E83">
-        <v>0.5017846629685156</v>
+        <v>0.5036699043994703</v>
       </c>
       <c r="F83">
-        <v>-1.781399465992843</v>
+        <v>-0.9980714370962516</v>
       </c>
     </row>
     <row r="84" spans="1:6">
@@ -2893,7 +2893,7 @@
         <v>310</v>
       </c>
       <c r="F85">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="86" spans="1:6">
@@ -2930,7 +2930,7 @@
         <v>310</v>
       </c>
       <c r="F87">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="88" spans="1:6">
@@ -2938,19 +2938,19 @@
         <v>92</v>
       </c>
       <c r="B88">
-        <v>0.4048929734959118</v>
+        <v>0.3908876216611158</v>
       </c>
       <c r="C88">
-        <v>0.6670239410004091</v>
+        <v>0.6277874687749131</v>
       </c>
       <c r="D88">
-        <v>0.5942571847129068</v>
+        <v>0.5899970024324156</v>
       </c>
       <c r="E88">
-        <v>0.4449209378677172</v>
+        <v>0.3941171059508125</v>
       </c>
       <c r="F88">
-        <v>-0.2690432017813032</v>
+        <v>-0.2899180272882586</v>
       </c>
     </row>
     <row r="89" spans="1:6">
@@ -2987,7 +2987,7 @@
         <v>310</v>
       </c>
       <c r="F90">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="91" spans="1:6">
@@ -3007,7 +3007,7 @@
         <v>310</v>
       </c>
       <c r="F91">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="92" spans="1:6">
@@ -3015,19 +3015,19 @@
         <v>96</v>
       </c>
       <c r="B92">
-        <v>0.304568631417102</v>
+        <v>0.2940048025831061</v>
       </c>
       <c r="C92">
-        <v>0.479428157013733</v>
+        <v>0.481265861150953</v>
       </c>
       <c r="D92">
-        <v>0.4127569378140264</v>
+        <v>0.4048734936493484</v>
       </c>
       <c r="E92">
-        <v>0.2298513577375846</v>
+        <v>0.2316168291093684</v>
       </c>
       <c r="F92">
-        <v>8.429547159269022</v>
+        <v>16.58943149519954</v>
       </c>
     </row>
     <row r="93" spans="1:6">
@@ -3035,16 +3035,16 @@
         <v>97</v>
       </c>
       <c r="B93">
-        <v>0.8607614056538685</v>
+        <v>0.8596292344952952</v>
       </c>
       <c r="C93">
-        <v>1.06485287690935</v>
+        <v>1.064584642892928</v>
       </c>
       <c r="D93">
-        <v>0.9403051268411277</v>
+        <v>0.939253630497371</v>
       </c>
       <c r="E93">
-        <v>1.13391164946212</v>
+        <v>1.133340461883464</v>
       </c>
       <c r="F93">
         <v>-6</v>
@@ -3067,7 +3067,7 @@
         <v>310</v>
       </c>
       <c r="F94">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="95" spans="1:6">
@@ -3087,7 +3087,7 @@
         <v>310</v>
       </c>
       <c r="F95">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="96" spans="1:6">
@@ -3095,19 +3095,19 @@
         <v>100</v>
       </c>
       <c r="B96">
-        <v>0.2066781557564579</v>
+        <v>0.2093525242294649</v>
       </c>
       <c r="C96">
-        <v>0.3280818010964017</v>
+        <v>0.3644898683339252</v>
       </c>
       <c r="D96">
-        <v>0.2917003785683318</v>
+        <v>0.2927934166100877</v>
       </c>
       <c r="E96">
-        <v>0.1076376682106589</v>
+        <v>0.1328528641180821</v>
       </c>
       <c r="F96">
-        <v>0.663537194112052</v>
+        <v>0.5720604443017498</v>
       </c>
     </row>
     <row r="97" spans="1:6">
@@ -3115,19 +3115,19 @@
         <v>101</v>
       </c>
       <c r="B97">
-        <v>0.3995148892813217</v>
+        <v>0.4129033550775977</v>
       </c>
       <c r="C97">
-        <v>0.541914593025275</v>
+        <v>0.5410872520335229</v>
       </c>
       <c r="D97">
-        <v>0.4853952048767886</v>
+        <v>0.495581595136489</v>
       </c>
       <c r="E97">
-        <v>0.2936714261337495</v>
+        <v>0.2927754143131892</v>
       </c>
       <c r="F97">
-        <v>1.569587059225095</v>
+        <v>1.85685438658264</v>
       </c>
     </row>
     <row r="98" spans="1:6">
@@ -3135,19 +3135,19 @@
         <v>102</v>
       </c>
       <c r="B98">
-        <v>0.0959979654513925</v>
+        <v>0.04062203772979749</v>
       </c>
       <c r="C98">
-        <v>0.2261774807012937</v>
+        <v>0.09825603165048437</v>
       </c>
       <c r="D98">
-        <v>0.2194219432740467</v>
+        <v>0.09819355606053182</v>
       </c>
       <c r="E98">
-        <v>0.05115625277638407</v>
+        <v>0.009654247755700986</v>
       </c>
       <c r="F98">
-        <v>-0.5000946416553391</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="99" spans="1:6">
@@ -3155,19 +3155,19 @@
         <v>103</v>
       </c>
       <c r="B99">
-        <v>0.4138431593001325</v>
+        <v>0.4281706528120228</v>
       </c>
       <c r="C99">
-        <v>0.5988750989994065</v>
+        <v>0.5996992102796563</v>
       </c>
       <c r="D99">
-        <v>0.5338176004310126</v>
+        <v>0.5373824318200151</v>
       </c>
       <c r="E99">
-        <v>0.358651384201549</v>
+        <v>0.3596391428100434</v>
       </c>
       <c r="F99">
-        <v>0.1906923089634756</v>
+        <v>-0.7692101453925905</v>
       </c>
     </row>
     <row r="100" spans="1:6">
@@ -3192,19 +3192,19 @@
         <v>105</v>
       </c>
       <c r="B101">
-        <v>0.7905610175154597</v>
+        <v>0.5105201999310677</v>
       </c>
       <c r="C101">
-        <v>1.354485281112222</v>
+        <v>1.053329170153695</v>
       </c>
       <c r="D101">
-        <v>1.130191421028194</v>
+        <v>0.890296642952612</v>
       </c>
       <c r="E101">
-        <v>1.834630376749656</v>
+        <v>1.109502340696671</v>
       </c>
       <c r="F101">
-        <v>-110.8725674641125</v>
+        <v>92.31336583498974</v>
       </c>
     </row>
     <row r="102" spans="1:6">
@@ -3212,39 +3212,39 @@
         <v>106</v>
       </c>
       <c r="B102">
-        <v>0.4482548978394882</v>
+        <v>0.4561762077511383</v>
       </c>
       <c r="C102">
-        <v>0.574827861100393</v>
+        <v>0.7280685052782682</v>
       </c>
       <c r="D102">
-        <v>0.5280780560635069</v>
+        <v>0.5833843374952914</v>
       </c>
       <c r="E102">
-        <v>0.3304270698972526</v>
+        <v>0.5300837483781315</v>
       </c>
       <c r="F102">
-        <v>-66.92009493873735</v>
+        <v>8.831344399212295</v>
       </c>
     </row>
     <row r="103" spans="1:6">
       <c r="A103" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="B103" t="s">
-        <v>310</v>
-      </c>
-      <c r="C103" t="s">
-        <v>310</v>
-      </c>
-      <c r="D103" t="s">
-        <v>310</v>
-      </c>
-      <c r="E103" t="s">
-        <v>310</v>
+      <c r="B103">
+        <v>0.4983840035848606</v>
+      </c>
+      <c r="C103">
+        <v>0.8315997480765458</v>
+      </c>
+      <c r="D103">
+        <v>0.7121725497295712</v>
+      </c>
+      <c r="E103">
+        <v>0.6915581410009745</v>
       </c>
       <c r="F103">
-        <v>0</v>
+        <v>-43.08256670427438</v>
       </c>
     </row>
     <row r="104" spans="1:6">
@@ -3264,7 +3264,7 @@
         <v>310</v>
       </c>
       <c r="F104">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="105" spans="1:6">
@@ -3284,7 +3284,7 @@
         <v>310</v>
       </c>
       <c r="F105">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="106" spans="1:6">
@@ -3304,7 +3304,7 @@
         <v>310</v>
       </c>
       <c r="F106">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="107" spans="1:6">
@@ -3324,7 +3324,7 @@
         <v>310</v>
       </c>
       <c r="F107">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="108" spans="1:6">
@@ -3366,19 +3366,19 @@
         <v>114</v>
       </c>
       <c r="B110">
-        <v>0.5784387198978956</v>
+        <v>0.5645200460247454</v>
       </c>
       <c r="C110">
-        <v>1.093432591498439</v>
+        <v>1.088749779461873</v>
       </c>
       <c r="D110">
-        <v>0.9774555384886235</v>
+        <v>0.9661567016221634</v>
       </c>
       <c r="E110">
-        <v>1.195594832150992</v>
+        <v>1.185376082278277</v>
       </c>
       <c r="F110">
-        <v>2.10741480328674</v>
+        <v>2.530344307306393</v>
       </c>
     </row>
     <row r="111" spans="1:6">
@@ -3386,19 +3386,19 @@
         <v>115</v>
       </c>
       <c r="B111">
-        <v>0.4398361832922741</v>
+        <v>0.4416554352546634</v>
       </c>
       <c r="C111">
-        <v>0.6593216584557064</v>
+        <v>0.6589010706372558</v>
       </c>
       <c r="D111">
-        <v>0.583558755109578</v>
+        <v>0.5899633496432086</v>
       </c>
       <c r="E111">
-        <v>0.4347050493087832</v>
+        <v>0.434150620886922</v>
       </c>
       <c r="F111">
-        <v>-2.086322628931795</v>
+        <v>-1.688485570771818</v>
       </c>
     </row>
     <row r="112" spans="1:6">
@@ -3406,19 +3406,19 @@
         <v>116</v>
       </c>
       <c r="B112">
-        <v>0.8241114646178116</v>
+        <v>0.8464165901966925</v>
       </c>
       <c r="C112">
-        <v>1.56059129648827</v>
+        <v>1.55988990911498</v>
       </c>
       <c r="D112">
-        <v>1.23732143602911</v>
+        <v>1.376639881629342</v>
       </c>
       <c r="E112">
-        <v>2.43544519467494</v>
+        <v>2.433256528558741</v>
       </c>
       <c r="F112">
-        <v>0.2052042783915634</v>
+        <v>2.394687067547814</v>
       </c>
     </row>
     <row r="113" spans="1:6">
@@ -3438,7 +3438,7 @@
         <v>310</v>
       </c>
       <c r="F113">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="114" spans="1:6">
@@ -3458,7 +3458,7 @@
         <v>310</v>
       </c>
       <c r="F114">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="115" spans="1:6">
@@ -3478,7 +3478,7 @@
         <v>310</v>
       </c>
       <c r="F115">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="116" spans="1:6">
@@ -3515,27 +3515,27 @@
         <v>310</v>
       </c>
       <c r="F117">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="118" spans="1:6">
       <c r="A118" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="B118" t="s">
-        <v>310</v>
-      </c>
-      <c r="C118" t="s">
-        <v>310</v>
-      </c>
-      <c r="D118" t="s">
-        <v>310</v>
-      </c>
-      <c r="E118" t="s">
-        <v>310</v>
+      <c r="B118">
+        <v>0.3983281184294905</v>
+      </c>
+      <c r="C118">
+        <v>0.6934139699784225</v>
+      </c>
+      <c r="D118">
+        <v>0.5253393933990378</v>
+      </c>
+      <c r="E118">
+        <v>0.4808229337612367</v>
       </c>
       <c r="F118">
-        <v>0</v>
+        <v>16.68494473029007</v>
       </c>
     </row>
     <row r="119" spans="1:6">
@@ -3543,19 +3543,19 @@
         <v>123</v>
       </c>
       <c r="B119">
-        <v>0.3185657790423642</v>
+        <v>0.3293122110983625</v>
       </c>
       <c r="C119">
-        <v>0.6441279431738579</v>
+        <v>0.6035120488189097</v>
       </c>
       <c r="D119">
-        <v>0.4311621005620977</v>
+        <v>0.4384791255709587</v>
       </c>
       <c r="E119">
-        <v>0.4149008071773847</v>
+        <v>0.3642267930695981</v>
       </c>
       <c r="F119">
-        <v>6.027855505961034</v>
+        <v>2.763254971884861</v>
       </c>
     </row>
     <row r="120" spans="1:6">
@@ -3563,19 +3563,19 @@
         <v>124</v>
       </c>
       <c r="B120">
-        <v>0.4982561542508095</v>
+        <v>0.5149209260341896</v>
       </c>
       <c r="C120">
-        <v>0.8450188528743929</v>
+        <v>0.8457767186794463</v>
       </c>
       <c r="D120">
-        <v>0.7038404417040953</v>
+        <v>0.7062432187338327</v>
       </c>
       <c r="E120">
-        <v>0.7140568617131549</v>
+        <v>0.7153382578601712</v>
       </c>
       <c r="F120">
-        <v>-36.73992125160704</v>
+        <v>-55.48042807498611</v>
       </c>
     </row>
     <row r="121" spans="1:6">
@@ -3583,19 +3583,19 @@
         <v>125</v>
       </c>
       <c r="B121">
-        <v>0.4845793070395378</v>
+        <v>0.486246418106691</v>
       </c>
       <c r="C121">
-        <v>0.7493403030970116</v>
+        <v>0.7507347341801097</v>
       </c>
       <c r="D121">
-        <v>0.5746875532525267</v>
+        <v>0.5765864963799529</v>
       </c>
       <c r="E121">
-        <v>0.5615108898455212</v>
+        <v>0.56360264110448</v>
       </c>
       <c r="F121">
-        <v>-42.17629166563714</v>
+        <v>-42.44781588998229</v>
       </c>
     </row>
     <row r="122" spans="1:6">
@@ -3603,39 +3603,39 @@
         <v>126</v>
       </c>
       <c r="B122">
-        <v>0.4236932930186926</v>
+        <v>0.4321167935986103</v>
       </c>
       <c r="C122">
-        <v>0.7177711058006965</v>
+        <v>0.6953320888161367</v>
       </c>
       <c r="D122">
-        <v>0.5993263352291045</v>
+        <v>0.5936353167253385</v>
       </c>
       <c r="E122">
-        <v>0.5151953603223547</v>
+        <v>0.4834867137374119</v>
       </c>
       <c r="F122">
-        <v>10.58245849604561</v>
+        <v>0.630460465506994</v>
       </c>
     </row>
     <row r="123" spans="1:6">
       <c r="A123" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="B123" t="s">
-        <v>310</v>
-      </c>
-      <c r="C123" t="s">
-        <v>310</v>
-      </c>
-      <c r="D123" t="s">
-        <v>310</v>
-      </c>
-      <c r="E123" t="s">
-        <v>310</v>
+      <c r="B123">
+        <v>0.8167835248593663</v>
+      </c>
+      <c r="C123">
+        <v>1.864704475857514</v>
+      </c>
+      <c r="D123">
+        <v>1.446661464603421</v>
+      </c>
+      <c r="E123">
+        <v>3.477122782283047</v>
       </c>
       <c r="F123">
-        <v>0</v>
+        <v>-48.52423467976927</v>
       </c>
     </row>
     <row r="124" spans="1:6">
@@ -3655,7 +3655,7 @@
         <v>310</v>
       </c>
       <c r="F124">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="125" spans="1:6">
@@ -3675,7 +3675,7 @@
         <v>310</v>
       </c>
       <c r="F125">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="126" spans="1:6">
@@ -3695,7 +3695,7 @@
         <v>310</v>
       </c>
       <c r="F126">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="127" spans="1:6">
@@ -3703,19 +3703,19 @@
         <v>131</v>
       </c>
       <c r="B127">
-        <v>0.3129624227609594</v>
+        <v>0.2959515733676739</v>
       </c>
       <c r="C127">
-        <v>0.5596353528767318</v>
+        <v>0.566880109241846</v>
       </c>
       <c r="D127">
-        <v>0.4163336963218371</v>
+        <v>0.4043719840201772</v>
       </c>
       <c r="E127">
-        <v>0.3131917281894641</v>
+        <v>0.3213530582540472</v>
       </c>
       <c r="F127">
-        <v>-4.636136775466693</v>
+        <v>2.930281906165798</v>
       </c>
     </row>
     <row r="128" spans="1:6">
@@ -3723,19 +3723,19 @@
         <v>132</v>
       </c>
       <c r="B128">
-        <v>0.3813301772104858</v>
+        <v>0.3216772400051488</v>
       </c>
       <c r="C128">
-        <v>0.6646374117066404</v>
+        <v>0.4941748759493278</v>
       </c>
       <c r="D128">
-        <v>0.4903329992376443</v>
+        <v>0.4094100108648521</v>
       </c>
       <c r="E128">
-        <v>0.4417428890401022</v>
+        <v>0.2442088080195335</v>
       </c>
       <c r="F128">
-        <v>4.92977698610111</v>
+        <v>-7.875367317453819</v>
       </c>
     </row>
     <row r="129" spans="1:6">
@@ -3755,7 +3755,7 @@
         <v>310</v>
       </c>
       <c r="F129">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="130" spans="1:6">
@@ -3775,7 +3775,7 @@
         <v>310</v>
       </c>
       <c r="F130">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="131" spans="1:6">
@@ -3851,19 +3851,19 @@
         <v>139</v>
       </c>
       <c r="B135">
-        <v>0.06896693874977081</v>
+        <v>0.0728815751226672</v>
       </c>
       <c r="C135">
-        <v>1.120464319247908</v>
+        <v>1.106907303192051</v>
       </c>
       <c r="D135">
-        <v>0.8238565390537147</v>
+        <v>0.8732870546719509</v>
       </c>
       <c r="E135">
-        <v>1.255440290707677</v>
+        <v>1.225243777859899</v>
       </c>
       <c r="F135">
-        <v>0.6840329100134637</v>
+        <v>0.5437927878897018</v>
       </c>
     </row>
     <row r="136" spans="1:6">
@@ -3888,19 +3888,19 @@
         <v>141</v>
       </c>
       <c r="B137">
-        <v>0.385820589678651</v>
+        <v>0.4160288442211611</v>
       </c>
       <c r="C137">
-        <v>0.6648184042027456</v>
+        <v>0.7089957860678451</v>
       </c>
       <c r="D137">
-        <v>0.5065571664610358</v>
+        <v>0.5296443083273544</v>
       </c>
       <c r="E137">
-        <v>0.4419835105666852</v>
+        <v>0.5026750246619616</v>
       </c>
       <c r="F137">
-        <v>3.685561942328552</v>
+        <v>-7.171029728375871</v>
       </c>
     </row>
     <row r="138" spans="1:6">
@@ -3908,19 +3908,19 @@
         <v>142</v>
       </c>
       <c r="B138">
-        <v>0.4006094965923148</v>
+        <v>0.40367939593658</v>
       </c>
       <c r="C138">
-        <v>2.110457350790217</v>
+        <v>2.109259525237448</v>
       </c>
       <c r="D138">
-        <v>1.652748608162935</v>
+        <v>1.652717972190275</v>
       </c>
       <c r="E138">
-        <v>4.454030229504459</v>
+        <v>4.448975744804903</v>
       </c>
       <c r="F138">
-        <v>-0.4264732931894981</v>
+        <v>-1.005587426792496</v>
       </c>
     </row>
     <row r="139" spans="1:6">
@@ -3928,19 +3928,19 @@
         <v>143</v>
       </c>
       <c r="B139">
-        <v>0.3563016139165351</v>
+        <v>0.3611508861465075</v>
       </c>
       <c r="C139">
-        <v>0.6445236311607461</v>
+        <v>0.5840524650962906</v>
       </c>
       <c r="D139">
-        <v>0.4966996687421567</v>
+        <v>0.4952618399557535</v>
       </c>
       <c r="E139">
-        <v>0.4154107111246334</v>
+        <v>0.3411172819850537</v>
       </c>
       <c r="F139">
-        <v>0.2956916700642247</v>
+        <v>-0.5945557011303575</v>
       </c>
     </row>
     <row r="140" spans="1:6">
@@ -3948,19 +3948,19 @@
         <v>144</v>
       </c>
       <c r="B140">
-        <v>0.4853651078282456</v>
+        <v>0.4882258376264948</v>
       </c>
       <c r="C140">
-        <v>0.5884215270626194</v>
+        <v>0.5897986188687835</v>
       </c>
       <c r="D140">
-        <v>0.5259482608248239</v>
+        <v>0.5281760599275238</v>
       </c>
       <c r="E140">
-        <v>0.3462398935107049</v>
+        <v>0.3478624108195245</v>
       </c>
       <c r="F140">
-        <v>-5.577062745444993</v>
+        <v>-5.626584835822298</v>
       </c>
     </row>
     <row r="141" spans="1:6">
@@ -3968,19 +3968,19 @@
         <v>145</v>
       </c>
       <c r="B141">
-        <v>0.2525546389922634</v>
+        <v>0.1492441936718076</v>
       </c>
       <c r="C141">
-        <v>0.39124137381816</v>
+        <v>0.5329032933134091</v>
       </c>
       <c r="D141">
-        <v>0.289544468316058</v>
+        <v>0.2945947021148457</v>
       </c>
       <c r="E141">
-        <v>0.1530698125871212</v>
+        <v>0.2839859200242774</v>
       </c>
       <c r="F141">
-        <v>-3.422949375998117</v>
+        <v>6.532401925372981</v>
       </c>
     </row>
     <row r="142" spans="1:6">
@@ -4000,27 +4000,27 @@
         <v>310</v>
       </c>
       <c r="F142">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="143" spans="1:6">
       <c r="A143" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="B143" t="s">
-        <v>310</v>
-      </c>
-      <c r="C143" t="s">
-        <v>310</v>
-      </c>
-      <c r="D143" t="s">
-        <v>310</v>
-      </c>
-      <c r="E143" t="s">
-        <v>310</v>
+      <c r="B143">
+        <v>0.6438160808098027</v>
+      </c>
+      <c r="C143">
+        <v>1.214455045063729</v>
+      </c>
+      <c r="D143">
+        <v>0.9646229105222818</v>
+      </c>
+      <c r="E143">
+        <v>1.474901056480745</v>
       </c>
       <c r="F143">
-        <v>0</v>
+        <v>-20.60128958527145</v>
       </c>
     </row>
     <row r="144" spans="1:6">
@@ -4028,19 +4028,19 @@
         <v>148</v>
       </c>
       <c r="B144">
-        <v>0.5010457360767278</v>
+        <v>0.4633547942434532</v>
       </c>
       <c r="C144">
-        <v>0.8624480842164173</v>
+        <v>0.856624416416393</v>
       </c>
       <c r="D144">
-        <v>0.7456018940627953</v>
+        <v>0.7296403262879196</v>
       </c>
       <c r="E144">
-        <v>0.7438166979685684</v>
+        <v>0.7338053908007258</v>
       </c>
       <c r="F144">
-        <v>-8.83307260942501</v>
+        <v>33.60344407382006</v>
       </c>
     </row>
     <row r="145" spans="1:6">
@@ -4048,39 +4048,39 @@
         <v>149</v>
       </c>
       <c r="B145">
-        <v>0.4511306363976431</v>
+        <v>0.4531350950967126</v>
       </c>
       <c r="C145">
-        <v>0.7165107413155285</v>
+        <v>0.7181104033976367</v>
       </c>
       <c r="D145">
-        <v>0.5607760666547537</v>
+        <v>0.5625147023949431</v>
       </c>
       <c r="E145">
-        <v>0.5133876424205281</v>
+        <v>0.5156825514679164</v>
       </c>
       <c r="F145">
-        <v>-0.8716088498943823</v>
+        <v>-0.8888391551000644</v>
       </c>
     </row>
     <row r="146" spans="1:6">
       <c r="A146" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="B146" t="s">
-        <v>310</v>
-      </c>
-      <c r="C146" t="s">
-        <v>310</v>
-      </c>
-      <c r="D146" t="s">
-        <v>310</v>
-      </c>
-      <c r="E146" t="s">
-        <v>310</v>
+      <c r="B146">
+        <v>0.4338659476839547</v>
+      </c>
+      <c r="C146">
+        <v>0.8533491099792843</v>
+      </c>
+      <c r="D146">
+        <v>0.7319764229721674</v>
+      </c>
+      <c r="E146">
+        <v>0.7282047035024366</v>
       </c>
       <c r="F146">
-        <v>0</v>
+        <v>75.36767588768225</v>
       </c>
     </row>
     <row r="147" spans="1:6">
@@ -4088,19 +4088,19 @@
         <v>151</v>
       </c>
       <c r="B147">
-        <v>0.5005646484258532</v>
+        <v>0.7653652464105655</v>
       </c>
       <c r="C147">
-        <v>0.8225053173938046</v>
+        <v>1.338888539476562</v>
       </c>
       <c r="D147">
-        <v>0.7174537779852038</v>
+        <v>1.101549660718926</v>
       </c>
       <c r="E147">
-        <v>0.6765149971410832</v>
+        <v>1.792622521141681</v>
       </c>
       <c r="F147">
-        <v>-6.934687174740843</v>
+        <v>-11.4582357796715</v>
       </c>
     </row>
     <row r="148" spans="1:6">
@@ -4108,19 +4108,19 @@
         <v>152</v>
       </c>
       <c r="B148">
-        <v>1.150676562057832</v>
+        <v>1.275889004184602</v>
       </c>
       <c r="C148">
-        <v>3.323994298993534</v>
+        <v>2.859485626930054</v>
       </c>
       <c r="D148">
-        <v>2.559772491813647</v>
+        <v>2.465347523562167</v>
       </c>
       <c r="E148">
-        <v>11.04893809974151</v>
+        <v>8.176658050619567</v>
       </c>
       <c r="F148">
-        <v>11.91410068089244</v>
+        <v>-36.6858457824888</v>
       </c>
     </row>
     <row r="149" spans="1:6">
@@ -4128,19 +4128,19 @@
         <v>153</v>
       </c>
       <c r="B149">
-        <v>0.4918312464860038</v>
+        <v>0.4918538407601151</v>
       </c>
       <c r="C149">
-        <v>0.9212514352609384</v>
+        <v>0.9212487727669947</v>
       </c>
       <c r="D149">
-        <v>0.7359393978213535</v>
+        <v>0.7359567666480857</v>
       </c>
       <c r="E149">
-        <v>0.8487042069703391</v>
+        <v>0.8486993013246938</v>
       </c>
       <c r="F149">
-        <v>10.24366700244382</v>
+        <v>10.22204641208251</v>
       </c>
     </row>
     <row r="150" spans="1:6">
@@ -4160,7 +4160,7 @@
         <v>310</v>
       </c>
       <c r="F150">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="151" spans="1:6">
@@ -4168,16 +4168,16 @@
         <v>155</v>
       </c>
       <c r="B151">
-        <v>0.0009082223457227423</v>
+        <v>0.00402614097617741</v>
       </c>
       <c r="C151">
-        <v>0.002265666427952374</v>
+        <v>0.01006040287588094</v>
       </c>
       <c r="D151">
-        <v>0.001948517310966791</v>
+        <v>0.009954253967204618</v>
       </c>
       <c r="E151">
-        <v>5.133244362750469E-06</v>
+        <v>0.0001012117060250334</v>
       </c>
       <c r="F151">
         <v>2</v>
@@ -4188,19 +4188,19 @@
         <v>156</v>
       </c>
       <c r="B152">
-        <v>0.4791234899029858</v>
+        <v>0.4790419534912399</v>
       </c>
       <c r="C152">
-        <v>0.7373721973820458</v>
+        <v>0.7409104321407584</v>
       </c>
       <c r="D152">
-        <v>0.6277460990475878</v>
+        <v>0.6280438166645673</v>
       </c>
       <c r="E152">
-        <v>0.5437177574720268</v>
+        <v>0.5489482684550052</v>
       </c>
       <c r="F152">
-        <v>-1.442603317359418</v>
+        <v>-1.359610690572456</v>
       </c>
     </row>
     <row r="153" spans="1:6">
@@ -4208,19 +4208,19 @@
         <v>157</v>
       </c>
       <c r="B153">
-        <v>0.8628150737819645</v>
+        <v>0.8724468677720507</v>
       </c>
       <c r="C153">
-        <v>1.017765347308489</v>
+        <v>1.033885267446795</v>
       </c>
       <c r="D153">
-        <v>1.01407909854428</v>
+        <v>1.032197449551926</v>
       </c>
       <c r="E153">
-        <v>1.035846302181968</v>
+        <v>1.068918746243531</v>
       </c>
       <c r="F153">
-        <v>-1.210032827070909</v>
+        <v>-1.142790430076464</v>
       </c>
     </row>
     <row r="154" spans="1:6">
@@ -4240,7 +4240,7 @@
         <v>310</v>
       </c>
       <c r="F154">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="155" spans="1:6">
@@ -4248,19 +4248,19 @@
         <v>159</v>
       </c>
       <c r="B155">
-        <v>0.4928357689241054</v>
+        <v>0.5288802692061396</v>
       </c>
       <c r="C155">
-        <v>0.8005284863898273</v>
+        <v>0.8362518131740214</v>
       </c>
       <c r="D155">
-        <v>0.6938461974921344</v>
+        <v>0.7109006029495013</v>
       </c>
       <c r="E155">
-        <v>0.640845857521588</v>
+        <v>0.6993170950368384</v>
       </c>
       <c r="F155">
-        <v>-23.40330934207978</v>
+        <v>-52.34396035367549</v>
       </c>
     </row>
     <row r="156" spans="1:6">
@@ -4268,19 +4268,19 @@
         <v>160</v>
       </c>
       <c r="B156">
-        <v>0.04012249054896399</v>
+        <v>0.02977187499790068</v>
       </c>
       <c r="C156">
-        <v>1.438748961282567</v>
+        <v>0.9635399800457857</v>
       </c>
       <c r="D156">
-        <v>1.082939375101477</v>
+        <v>0.7761694289898574</v>
       </c>
       <c r="E156">
-        <v>2.069998573591666</v>
+        <v>0.9284092931466331</v>
       </c>
       <c r="F156">
-        <v>-0.8275372160535753</v>
+        <v>-2.055048014206355</v>
       </c>
     </row>
     <row r="157" spans="1:6">
@@ -4317,7 +4317,7 @@
         <v>310</v>
       </c>
       <c r="F158">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="159" spans="1:6">
@@ -4337,7 +4337,7 @@
         <v>310</v>
       </c>
       <c r="F159">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="160" spans="1:6">
@@ -4345,19 +4345,19 @@
         <v>164</v>
       </c>
       <c r="B160">
-        <v>0.3615516700105582</v>
+        <v>0.3527024109402015</v>
       </c>
       <c r="C160">
-        <v>0.575129020540661</v>
+        <v>0.5567305481507143</v>
       </c>
       <c r="D160">
-        <v>0.4503671935852196</v>
+        <v>0.4375575297644098</v>
       </c>
       <c r="E160">
-        <v>0.33077339026806</v>
+        <v>0.3099489032441949</v>
       </c>
       <c r="F160">
-        <v>-2.449541840719177</v>
+        <v>-1.939093165465328</v>
       </c>
     </row>
     <row r="161" spans="1:6">
@@ -4365,19 +4365,19 @@
         <v>165</v>
       </c>
       <c r="B161">
-        <v>0.3169215864337664</v>
+        <v>0.3308681696525628</v>
       </c>
       <c r="C161">
-        <v>0.6777656561589916</v>
+        <v>0.516280116682824</v>
       </c>
       <c r="D161">
-        <v>0.459378504770464</v>
+        <v>0.4668620059497416</v>
       </c>
       <c r="E161">
-        <v>0.4593662846686286</v>
+        <v>0.2665451588820305</v>
       </c>
       <c r="F161">
-        <v>41.3786256645903</v>
+        <v>28.40988167825193</v>
       </c>
     </row>
     <row r="162" spans="1:6">
@@ -4385,19 +4385,19 @@
         <v>166</v>
       </c>
       <c r="B162">
-        <v>0.4946676129514505</v>
+        <v>0.207778818160159</v>
       </c>
       <c r="C162">
-        <v>0.8625583214359294</v>
+        <v>0.5803920215465137</v>
       </c>
       <c r="D162">
-        <v>0.6893018181027453</v>
+        <v>0.3475899393662734</v>
       </c>
       <c r="E162">
-        <v>0.744006857878368</v>
+        <v>0.3368548986748488</v>
       </c>
       <c r="F162">
-        <v>5.349600960085942</v>
+        <v>5.187977232459371</v>
       </c>
     </row>
     <row r="163" spans="1:6">
@@ -4405,19 +4405,19 @@
         <v>167</v>
       </c>
       <c r="B163">
-        <v>0.106654021425567</v>
+        <v>0.1704775222475092</v>
       </c>
       <c r="C163">
-        <v>0.3280261632800416</v>
+        <v>0.4203592374945298</v>
       </c>
       <c r="D163">
-        <v>0.2531141309672815</v>
+        <v>0.3906373640910221</v>
       </c>
       <c r="E163">
-        <v>0.1076011637962245</v>
+        <v>0.1767018885469825</v>
       </c>
       <c r="F163">
-        <v>3.287892931796559</v>
+        <v>1.384192727742014</v>
       </c>
     </row>
     <row r="164" spans="1:6">
@@ -4476,19 +4476,19 @@
         <v>171</v>
       </c>
       <c r="B167">
-        <v>0.3403422766227524</v>
+        <v>0.382083742186318</v>
       </c>
       <c r="C167">
-        <v>0.5839395296145247</v>
+        <v>0.6104122425410913</v>
       </c>
       <c r="D167">
-        <v>0.4668018035585669</v>
+        <v>0.5062342689489234</v>
       </c>
       <c r="E167">
-        <v>0.3409853742464323</v>
+        <v>0.372603105844044</v>
       </c>
       <c r="F167">
-        <v>1.721467805619291</v>
+        <v>-7.380643464738307</v>
       </c>
     </row>
     <row r="168" spans="1:6">
@@ -4508,7 +4508,7 @@
         <v>310</v>
       </c>
       <c r="F168">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="169" spans="1:6">
@@ -4532,20 +4532,20 @@
       <c r="A170" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="B170">
-        <v>0.8383688323351304</v>
-      </c>
-      <c r="C170">
-        <v>1.88654636325633</v>
-      </c>
-      <c r="D170">
-        <v>1.535293679171851</v>
-      </c>
-      <c r="E170">
-        <v>3.559057180715685</v>
+      <c r="B170" t="s">
+        <v>310</v>
+      </c>
+      <c r="C170" t="s">
+        <v>310</v>
+      </c>
+      <c r="D170" t="s">
+        <v>310</v>
+      </c>
+      <c r="E170" t="s">
+        <v>310</v>
       </c>
       <c r="F170">
-        <v>-3.241948034016915</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="171" spans="1:6">
@@ -4553,19 +4553,19 @@
         <v>175</v>
       </c>
       <c r="B171">
-        <v>0.4876567217055107</v>
+        <v>0.4520544170623264</v>
       </c>
       <c r="C171">
-        <v>0.9081855556213293</v>
+        <v>0.8133268527632759</v>
       </c>
       <c r="D171">
-        <v>0.781803888077401</v>
+        <v>0.7104113116192661</v>
       </c>
       <c r="E171">
-        <v>0.8248010034392227</v>
+        <v>0.6615005694258155</v>
       </c>
       <c r="F171">
-        <v>42.11289861993166</v>
+        <v>41.38543091897508</v>
       </c>
     </row>
     <row r="172" spans="1:6">
@@ -4573,19 +4573,19 @@
         <v>176</v>
       </c>
       <c r="B172">
-        <v>0.1882699232216646</v>
+        <v>0.1898439720388583</v>
       </c>
       <c r="C172">
-        <v>0.5077091939822649</v>
+        <v>0.5097354801444125</v>
       </c>
       <c r="D172">
-        <v>0.2801130735926425</v>
+        <v>0.2814640939760751</v>
       </c>
       <c r="E172">
-        <v>0.2577686256541211</v>
+        <v>0.2598302597180547</v>
       </c>
       <c r="F172">
-        <v>67.98191019810373</v>
+        <v>67.56486378568177</v>
       </c>
     </row>
     <row r="173" spans="1:6">
@@ -4605,7 +4605,7 @@
         <v>310</v>
       </c>
       <c r="F173">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="174" spans="1:6">
@@ -4630,19 +4630,19 @@
         <v>179</v>
       </c>
       <c r="B175">
-        <v>0.3038466026301311</v>
+        <v>0.3295320490661283</v>
       </c>
       <c r="C175">
-        <v>0.5985594287937381</v>
+        <v>0.495451308100269</v>
       </c>
       <c r="D175">
-        <v>0.4059651092417463</v>
+        <v>0.4296063453206383</v>
       </c>
       <c r="E175">
-        <v>0.3582733897978861</v>
+        <v>0.2454719986982677</v>
       </c>
       <c r="F175">
-        <v>-4.248565701286677</v>
+        <v>-6.402014992744578</v>
       </c>
     </row>
     <row r="176" spans="1:6">
@@ -4662,7 +4662,7 @@
         <v>310</v>
       </c>
       <c r="F176">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="177" spans="1:6">
@@ -4687,19 +4687,19 @@
         <v>182</v>
       </c>
       <c r="B178">
-        <v>0.2140873386097044</v>
+        <v>0.2455030757205547</v>
       </c>
       <c r="C178">
-        <v>0.4520309816631775</v>
+        <v>0.4676854884706</v>
       </c>
       <c r="D178">
-        <v>0.3225129150984664</v>
+        <v>0.3530786812490934</v>
       </c>
       <c r="E178">
-        <v>0.2043320083833759</v>
+        <v>0.2187297161259837</v>
       </c>
       <c r="F178">
-        <v>29.30455736919537</v>
+        <v>20.19433675447413</v>
       </c>
     </row>
     <row r="179" spans="1:6">
@@ -4724,39 +4724,39 @@
         <v>184</v>
       </c>
       <c r="B180">
-        <v>0.41645296080946</v>
+        <v>0.416408052536656</v>
       </c>
       <c r="C180">
-        <v>0.7607514217833887</v>
+        <v>0.7613103093510984</v>
       </c>
       <c r="D180">
-        <v>0.5848416661245002</v>
+        <v>0.5855084217468209</v>
       </c>
       <c r="E180">
-        <v>0.5787427257454475</v>
+        <v>0.5795933871242652</v>
       </c>
       <c r="F180">
-        <v>9.400742996605763</v>
+        <v>9.742314899034504</v>
       </c>
     </row>
     <row r="181" spans="1:6">
       <c r="A181" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="B181">
-        <v>0.5041493227026562</v>
-      </c>
-      <c r="C181">
-        <v>1.074833526484458</v>
-      </c>
-      <c r="D181">
-        <v>0.8866668646743767</v>
-      </c>
-      <c r="E181">
-        <v>1.155267109655016</v>
+      <c r="B181" t="s">
+        <v>310</v>
+      </c>
+      <c r="C181" t="s">
+        <v>310</v>
+      </c>
+      <c r="D181" t="s">
+        <v>310</v>
+      </c>
+      <c r="E181" t="s">
+        <v>310</v>
       </c>
       <c r="F181">
-        <v>16.1536703474188</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="182" spans="1:6">
@@ -4764,19 +4764,19 @@
         <v>186</v>
       </c>
       <c r="B182">
-        <v>0.1424150746641139</v>
+        <v>0.1502984103312495</v>
       </c>
       <c r="C182">
-        <v>0.2643250160144935</v>
+        <v>0.2643829319010723</v>
       </c>
       <c r="D182">
-        <v>0.1999299865850593</v>
+        <v>0.2073180910331138</v>
       </c>
       <c r="E182">
-        <v>0.06986771409106222</v>
+        <v>0.06989833468060701</v>
       </c>
       <c r="F182">
-        <v>0.1027427577643243</v>
+        <v>-0.0956940727928145</v>
       </c>
     </row>
     <row r="183" spans="1:6">
@@ -4784,19 +4784,19 @@
         <v>187</v>
       </c>
       <c r="B183">
-        <v>0.3750131384155835</v>
+        <v>0.3751553942219349</v>
       </c>
       <c r="C183">
-        <v>0.7070919056666813</v>
+        <v>0.7070715030891718</v>
       </c>
       <c r="D183">
-        <v>0.5000110018949773</v>
+        <v>0.5002460783947963</v>
       </c>
       <c r="E183">
-        <v>0.4999789630593389</v>
+        <v>0.4999501104807807</v>
       </c>
       <c r="F183">
-        <v>-0.0001563803782545703</v>
+        <v>0.005270650336936794</v>
       </c>
     </row>
     <row r="184" spans="1:6">
@@ -4816,7 +4816,7 @@
         <v>310</v>
       </c>
       <c r="F184">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="185" spans="1:6">
@@ -4824,19 +4824,19 @@
         <v>189</v>
       </c>
       <c r="B185">
-        <v>0.4772692044861657</v>
+        <v>0.466881230108722</v>
       </c>
       <c r="C185">
-        <v>0.7022660819584488</v>
+        <v>0.6887759074916638</v>
       </c>
       <c r="D185">
-        <v>0.5875770726958346</v>
+        <v>0.5946978914002768</v>
       </c>
       <c r="E185">
-        <v>0.4931776498692706</v>
+        <v>0.474412250740965</v>
       </c>
       <c r="F185">
-        <v>-0.4323368281897627</v>
+        <v>0.9295389565890317</v>
       </c>
     </row>
     <row r="186" spans="1:6">
@@ -4856,7 +4856,7 @@
         <v>310</v>
       </c>
       <c r="F186">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="187" spans="1:6">
@@ -4876,7 +4876,7 @@
         <v>310</v>
       </c>
       <c r="F187">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="188" spans="1:6">
@@ -4884,19 +4884,19 @@
         <v>192</v>
       </c>
       <c r="B188">
-        <v>0.2199023673469361</v>
+        <v>0.2199462552395472</v>
       </c>
       <c r="C188">
-        <v>0.5834810666250634</v>
+        <v>0.5834915976611571</v>
       </c>
       <c r="D188">
-        <v>0.3404777609659737</v>
+        <v>0.3405320949157521</v>
       </c>
       <c r="E188">
-        <v>0.3404501551099217</v>
+        <v>0.3404624445411697</v>
       </c>
       <c r="F188">
-        <v>58.76465682968185</v>
+        <v>58.78574440363101</v>
       </c>
     </row>
     <row r="189" spans="1:6">
@@ -4904,19 +4904,19 @@
         <v>193</v>
       </c>
       <c r="B189">
-        <v>0.392516453000241</v>
+        <v>0.3857490201349978</v>
       </c>
       <c r="C189">
-        <v>0.6798090390309531</v>
+        <v>0.6847765212142709</v>
       </c>
       <c r="D189">
-        <v>0.50256528233377</v>
+        <v>0.4887074604203119</v>
       </c>
       <c r="E189">
-        <v>0.4621403295481879</v>
+        <v>0.4689188840063188</v>
       </c>
       <c r="F189">
-        <v>-2.833805743682393</v>
+        <v>-15.34095803159718</v>
       </c>
     </row>
     <row r="190" spans="1:6">
@@ -4924,19 +4924,19 @@
         <v>194</v>
       </c>
       <c r="B190">
-        <v>0.4967583486312738</v>
+        <v>0.5156046624601106</v>
       </c>
       <c r="C190">
-        <v>0.6761263155842392</v>
+        <v>0.6788342869535134</v>
       </c>
       <c r="D190">
-        <v>0.6262281223251238</v>
+        <v>0.6320501809316952</v>
       </c>
       <c r="E190">
-        <v>0.4571467946255182</v>
+        <v>0.4608159891436851</v>
       </c>
       <c r="F190">
-        <v>-1.211129244774318</v>
+        <v>-1.841430924996881</v>
       </c>
     </row>
     <row r="191" spans="1:6">
@@ -4944,19 +4944,19 @@
         <v>195</v>
       </c>
       <c r="B191">
-        <v>0.5186714087825611</v>
+        <v>0.5088491025098729</v>
       </c>
       <c r="C191">
-        <v>0.5222305444569072</v>
+        <v>0.5137828583270969</v>
       </c>
       <c r="D191">
-        <v>0.5186714087825611</v>
+        <v>0.5088491025098729</v>
       </c>
       <c r="E191">
-        <v>0.2727247415637577</v>
+        <v>0.2639728255107618</v>
       </c>
       <c r="F191">
-        <v>-1.283003196740871</v>
+        <v>-1.371592116409436</v>
       </c>
     </row>
     <row r="192" spans="1:6">
@@ -4964,19 +4964,19 @@
         <v>196</v>
       </c>
       <c r="B192">
-        <v>0.03926687800315811</v>
+        <v>0.03862624245444794</v>
       </c>
       <c r="C192">
-        <v>0.08091713582261567</v>
+        <v>0.07565904198777204</v>
       </c>
       <c r="D192">
-        <v>0.06138410192247858</v>
+        <v>0.05931523648290041</v>
       </c>
       <c r="E192">
-        <v>0.006547582869735631</v>
+        <v>0.005724290634507453</v>
       </c>
       <c r="F192">
-        <v>-5.361999312050888</v>
+        <v>-4.425045425403383</v>
       </c>
     </row>
     <row r="193" spans="1:6">
@@ -4996,7 +4996,7 @@
         <v>310</v>
       </c>
       <c r="F193">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="194" spans="1:6">
@@ -5016,7 +5016,7 @@
         <v>310</v>
       </c>
       <c r="F194">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="195" spans="1:6">
@@ -5058,19 +5058,19 @@
         <v>201</v>
       </c>
       <c r="B197">
-        <v>0.4438835507404313</v>
+        <v>0.4460909008581062</v>
       </c>
       <c r="C197">
-        <v>0.5822433253109188</v>
+        <v>0.5822973477093795</v>
       </c>
       <c r="D197">
-        <v>0.5226365440486886</v>
+        <v>0.5242162919352906</v>
       </c>
       <c r="E197">
-        <v>0.3390072898691165</v>
+        <v>0.339070201149378</v>
       </c>
       <c r="F197">
-        <v>0.08232004769568944</v>
+        <v>0.102178723105484</v>
       </c>
     </row>
     <row r="198" spans="1:6">
@@ -5090,7 +5090,7 @@
         <v>310</v>
       </c>
       <c r="F198">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="199" spans="1:6">
@@ -5098,19 +5098,19 @@
         <v>203</v>
       </c>
       <c r="B199">
-        <v>0.3548810078487012</v>
+        <v>0.3347694867112433</v>
       </c>
       <c r="C199">
-        <v>0.6702832930826162</v>
+        <v>0.4678331165152002</v>
       </c>
       <c r="D199">
-        <v>0.4690297528946167</v>
+        <v>0.4349736613994769</v>
       </c>
       <c r="E199">
-        <v>0.4492796929856764</v>
+        <v>0.2188678249083248</v>
       </c>
       <c r="F199">
-        <v>-5.191902838766295</v>
+        <v>-10.12991951564931</v>
       </c>
     </row>
     <row r="200" spans="1:6">
@@ -5135,19 +5135,19 @@
         <v>205</v>
       </c>
       <c r="B201">
-        <v>0.3804507763180456</v>
+        <v>0.3027416774081985</v>
       </c>
       <c r="C201">
-        <v>0.6793930783978339</v>
+        <v>0.5556523930231174</v>
       </c>
       <c r="D201">
-        <v>0.4833466305159748</v>
+        <v>0.4469668705587754</v>
       </c>
       <c r="E201">
-        <v>0.4615749549748853</v>
+        <v>0.308749581872317</v>
       </c>
       <c r="F201">
-        <v>-11.26842618622693</v>
+        <v>54.90147793978542</v>
       </c>
     </row>
     <row r="202" spans="1:6">
@@ -5155,19 +5155,19 @@
         <v>206</v>
       </c>
       <c r="B202">
-        <v>0.2404977815492403</v>
+        <v>0.1607364726042349</v>
       </c>
       <c r="C202">
-        <v>0.3323879130221021</v>
+        <v>0.4683768188864613</v>
       </c>
       <c r="D202">
-        <v>0.3149540730606155</v>
+        <v>0.2857394930633659</v>
       </c>
       <c r="E202">
-        <v>0.1104817247231885</v>
+        <v>0.2193768444702009</v>
       </c>
       <c r="F202">
-        <v>-0.2175416478810625</v>
+        <v>2.499189549670287</v>
       </c>
     </row>
     <row r="203" spans="1:6">
@@ -5175,19 +5175,19 @@
         <v>207</v>
       </c>
       <c r="B203">
-        <v>0.667652922449674</v>
+        <v>0.6853313677989405</v>
       </c>
       <c r="C203">
-        <v>1.248960604614158</v>
+        <v>1.368522168413014</v>
       </c>
       <c r="D203">
-        <v>1.190551276193786</v>
+        <v>1.28893819297097</v>
       </c>
       <c r="E203">
-        <v>1.559902591878163</v>
+        <v>1.872852925437857</v>
       </c>
       <c r="F203">
-        <v>1.588103732278896</v>
+        <v>2.024465895227271</v>
       </c>
     </row>
     <row r="204" spans="1:6">
@@ -5195,19 +5195,19 @@
         <v>208</v>
       </c>
       <c r="B204">
-        <v>0.2571946133925463</v>
+        <v>0.275277941641764</v>
       </c>
       <c r="C204">
-        <v>0.8530552306787232</v>
+        <v>0.8817031317372196</v>
       </c>
       <c r="D204">
-        <v>0.7660837628667987</v>
+        <v>0.7333533666126597</v>
       </c>
       <c r="E204">
-        <v>0.7277032265883296</v>
+        <v>0.7774004125152209</v>
       </c>
       <c r="F204">
-        <v>1.432885791247513</v>
+        <v>0.5001323961308765</v>
       </c>
     </row>
     <row r="205" spans="1:6">
@@ -5215,19 +5215,19 @@
         <v>209</v>
       </c>
       <c r="B205">
-        <v>0.4426040662390356</v>
+        <v>0.355997152803689</v>
       </c>
       <c r="C205">
-        <v>0.7178365779284986</v>
+        <v>0.5827113578553055</v>
       </c>
       <c r="D205">
-        <v>0.5313780580704887</v>
+        <v>0.464880948076822</v>
       </c>
       <c r="E205">
-        <v>0.5152893526120975</v>
+        <v>0.3395525265735738</v>
       </c>
       <c r="F205">
-        <v>-27.01291844124745</v>
+        <v>4.655639249240527</v>
       </c>
     </row>
     <row r="206" spans="1:6">
@@ -5235,19 +5235,19 @@
         <v>210</v>
       </c>
       <c r="B206">
-        <v>0.4273343406979223</v>
+        <v>0.2585379686047735</v>
       </c>
       <c r="C206">
-        <v>0.7069047828866775</v>
+        <v>0.5750637967970718</v>
       </c>
       <c r="D206">
-        <v>0.5352156974148761</v>
+        <v>0.4091256098958189</v>
       </c>
       <c r="E206">
-        <v>0.4997143720680606</v>
+        <v>0.3306983703866639</v>
       </c>
       <c r="F206">
-        <v>-7.075394148600325</v>
+        <v>46.55587560378071</v>
       </c>
     </row>
     <row r="207" spans="1:6">
@@ -5267,7 +5267,7 @@
         <v>310</v>
       </c>
       <c r="F207">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="208" spans="1:6">
@@ -5393,20 +5393,20 @@
       <c r="A215" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="B215" t="s">
-        <v>310</v>
-      </c>
-      <c r="C215" t="s">
-        <v>310</v>
-      </c>
-      <c r="D215" t="s">
-        <v>310</v>
-      </c>
-      <c r="E215" t="s">
-        <v>310</v>
+      <c r="B215">
+        <v>1.338175722609128</v>
+      </c>
+      <c r="C215">
+        <v>3.650317236826344</v>
+      </c>
+      <c r="D215">
+        <v>3.015146192630671</v>
+      </c>
+      <c r="E215">
+        <v>13.32481592947152</v>
       </c>
       <c r="F215">
-        <v>0</v>
+        <v>-60.98734900620677</v>
       </c>
     </row>
     <row r="216" spans="1:6">
@@ -5482,19 +5482,19 @@
         <v>224</v>
       </c>
       <c r="B220">
-        <v>0.4233923715082052</v>
+        <v>0.4295857330551133</v>
       </c>
       <c r="C220">
-        <v>0.5465860079749036</v>
+        <v>0.546675626952461</v>
       </c>
       <c r="D220">
-        <v>0.4896956225988968</v>
+        <v>0.4847272232226051</v>
       </c>
       <c r="E220">
-        <v>0.2987562641139414</v>
+        <v>0.2988542411038663</v>
       </c>
       <c r="F220">
-        <v>-42.43741031700846</v>
+        <v>-50.26977072375709</v>
       </c>
     </row>
     <row r="221" spans="1:6">
@@ -5514,7 +5514,7 @@
         <v>310</v>
       </c>
       <c r="F221">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="222" spans="1:6">
@@ -5619,7 +5619,7 @@
         <v>310</v>
       </c>
       <c r="F227">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="228" spans="1:6">
@@ -5644,19 +5644,19 @@
         <v>233</v>
       </c>
       <c r="B229">
-        <v>0.7574868792217198</v>
+        <v>0.5053349344674251</v>
       </c>
       <c r="C229">
-        <v>1.421334082934467</v>
+        <v>1.003894674783688</v>
       </c>
       <c r="D229">
-        <v>1.155656471129482</v>
+        <v>0.8342078180914646</v>
       </c>
       <c r="E229">
-        <v>2.020190575311162</v>
+        <v>1.007804518059047</v>
       </c>
       <c r="F229">
-        <v>-144.7390289801947</v>
+        <v>-6.781771473610105</v>
       </c>
     </row>
     <row r="230" spans="1:6">
@@ -5664,19 +5664,19 @@
         <v>234</v>
       </c>
       <c r="B230">
-        <v>0.5622184768040115</v>
+        <v>0.6619908257215892</v>
       </c>
       <c r="C230">
-        <v>1.334440281908415</v>
+        <v>1.481381078725962</v>
       </c>
       <c r="D230">
-        <v>1.04968293068918</v>
+        <v>1.147830047217528</v>
       </c>
       <c r="E230">
-        <v>1.780730865979809</v>
+        <v>2.194489900407294</v>
       </c>
       <c r="F230">
-        <v>60.59155254346731</v>
+        <v>-4.240034804232944</v>
       </c>
     </row>
     <row r="231" spans="1:6">
@@ -5718,19 +5718,19 @@
         <v>237</v>
       </c>
       <c r="B233">
-        <v>0.4148309667815075</v>
+        <v>0.4222878305566237</v>
       </c>
       <c r="C233">
-        <v>0.6705837454215873</v>
+        <v>0.6714283711275043</v>
       </c>
       <c r="D233">
-        <v>0.544482150176524</v>
+        <v>0.5480568174908654</v>
       </c>
       <c r="E233">
-        <v>0.4496825596236442</v>
+        <v>0.4508160575549336</v>
       </c>
       <c r="F233">
-        <v>0.1759362518458352</v>
+        <v>-0.3024717179891662</v>
       </c>
     </row>
     <row r="234" spans="1:6">
@@ -5755,19 +5755,19 @@
         <v>239</v>
       </c>
       <c r="B235">
-        <v>0.3869516734290651</v>
+        <v>0.356127122962099</v>
       </c>
       <c r="C235">
-        <v>0.6439009406925649</v>
+        <v>0.588052207592958</v>
       </c>
       <c r="D235">
-        <v>0.5046703818429737</v>
+        <v>0.4726283183503223</v>
       </c>
       <c r="E235">
-        <v>0.4146084214247699</v>
+        <v>0.3458053988549513</v>
       </c>
       <c r="F235">
-        <v>-0.00119062793799493</v>
+        <v>0.1024443070104988</v>
       </c>
     </row>
     <row r="236" spans="1:6">
@@ -5787,7 +5787,7 @@
         <v>310</v>
       </c>
       <c r="F236">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="237" spans="1:6">
@@ -5795,19 +5795,19 @@
         <v>241</v>
       </c>
       <c r="B237">
-        <v>1.121298000710984</v>
+        <v>1.124048840308024</v>
       </c>
       <c r="C237">
-        <v>2.667398073068088</v>
+        <v>2.668015543285268</v>
       </c>
       <c r="D237">
-        <v>2.078745493098515</v>
+        <v>2.071315415012749</v>
       </c>
       <c r="E237">
-        <v>7.115012480207346</v>
+        <v>7.118306939211783</v>
       </c>
       <c r="F237">
-        <v>-5.982292316161075</v>
+        <v>-9.288911492973247</v>
       </c>
     </row>
     <row r="238" spans="1:6">
@@ -5815,19 +5815,19 @@
         <v>242</v>
       </c>
       <c r="B238">
-        <v>1.211105841466198</v>
+        <v>1.326518163040675</v>
       </c>
       <c r="C238">
-        <v>2.532384567810723</v>
+        <v>3.387662649277652</v>
       </c>
       <c r="D238">
-        <v>2.264361241659235</v>
+        <v>2.677736412412147</v>
       </c>
       <c r="E238">
-        <v>6.412971599285901</v>
+        <v>11.47625822531088</v>
       </c>
       <c r="F238">
-        <v>-28.72165308745859</v>
+        <v>-9.451263997096184</v>
       </c>
     </row>
     <row r="239" spans="1:6">
@@ -5847,7 +5847,7 @@
         <v>310</v>
       </c>
       <c r="F239">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="240" spans="1:6">
@@ -5855,19 +5855,19 @@
         <v>244</v>
       </c>
       <c r="B240">
-        <v>0.2431807022435123</v>
+        <v>0.2504989487827823</v>
       </c>
       <c r="C240">
-        <v>0.3646743209184232</v>
+        <v>0.3655685815958511</v>
       </c>
       <c r="D240">
-        <v>0.2842512603181421</v>
+        <v>0.2897596052992779</v>
       </c>
       <c r="E240">
-        <v>0.1329873603373131</v>
+        <v>0.1336403878500024</v>
       </c>
       <c r="F240">
-        <v>-0.2374124442434782</v>
+        <v>-0.1608399076465077</v>
       </c>
     </row>
     <row r="241" spans="1:6">
@@ -5904,7 +5904,7 @@
         <v>310</v>
       </c>
       <c r="F242">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="243" spans="1:6">
@@ -5928,20 +5928,20 @@
       <c r="A244" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="B244" t="s">
-        <v>310</v>
-      </c>
-      <c r="C244" t="s">
-        <v>310</v>
-      </c>
-      <c r="D244" t="s">
-        <v>310</v>
-      </c>
-      <c r="E244" t="s">
-        <v>310</v>
+      <c r="B244">
+        <v>0.6427158162330199</v>
+      </c>
+      <c r="C244">
+        <v>1.325497900422533</v>
+      </c>
+      <c r="D244">
+        <v>1.059055241492913</v>
+      </c>
+      <c r="E244">
+        <v>1.756944684024543</v>
       </c>
       <c r="F244">
-        <v>0</v>
+        <v>-10.38921700562227</v>
       </c>
     </row>
     <row r="245" spans="1:6">
@@ -5949,19 +5949,19 @@
         <v>249</v>
       </c>
       <c r="B245">
-        <v>0.2830227635305691</v>
+        <v>0.2846930871934558</v>
       </c>
       <c r="C245">
-        <v>0.4807345734065244</v>
+        <v>0.4786144654511642</v>
       </c>
       <c r="D245">
-        <v>0.3951201543298064</v>
+        <v>0.3951439241698497</v>
       </c>
       <c r="E245">
-        <v>0.231105730068353</v>
+        <v>0.2290718065391036</v>
       </c>
       <c r="F245">
-        <v>12.63267418922888</v>
+        <v>12.67930586777994</v>
       </c>
     </row>
     <row r="246" spans="1:6">
@@ -5969,19 +5969,19 @@
         <v>250</v>
       </c>
       <c r="B246">
-        <v>0.2913573783975878</v>
+        <v>0.299485503792361</v>
       </c>
       <c r="C246">
-        <v>0.4681779061740662</v>
+        <v>0.467939970088637</v>
       </c>
       <c r="D246">
-        <v>0.3934246196756435</v>
+        <v>0.3997806349475991</v>
       </c>
       <c r="E246">
-        <v>0.2191905518295327</v>
+        <v>0.2189678156065545</v>
       </c>
       <c r="F246">
-        <v>3.886303763166191</v>
+        <v>0.3606693865356807</v>
       </c>
     </row>
     <row r="247" spans="1:6">
@@ -6052,7 +6052,7 @@
         <v>310</v>
       </c>
       <c r="F250">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="251" spans="1:6">
@@ -6093,20 +6093,20 @@
       <c r="A253" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="B253" t="s">
-        <v>310</v>
-      </c>
-      <c r="C253" t="s">
-        <v>310</v>
-      </c>
-      <c r="D253" t="s">
-        <v>310</v>
-      </c>
-      <c r="E253" t="s">
-        <v>310</v>
+      <c r="B253">
+        <v>1.770251864979433</v>
+      </c>
+      <c r="C253">
+        <v>4.159374336069514</v>
+      </c>
+      <c r="D253">
+        <v>3.497495054484847</v>
+      </c>
+      <c r="E253">
+        <v>17.30039486755371</v>
       </c>
       <c r="F253">
-        <v>0</v>
+        <v>-3.751004055693889</v>
       </c>
     </row>
     <row r="254" spans="1:6">
@@ -6114,39 +6114,39 @@
         <v>258</v>
       </c>
       <c r="B254">
-        <v>0.6766802735953625</v>
+        <v>1.028497775472641</v>
       </c>
       <c r="C254">
-        <v>2.554274363636968</v>
+        <v>2.345503362570807</v>
       </c>
       <c r="D254">
-        <v>1.916023945903103</v>
+        <v>1.990039799119614</v>
       </c>
       <c r="E254">
-        <v>6.524317524733036</v>
+        <v>5.501386023830964</v>
       </c>
       <c r="F254">
-        <v>151.7182920639475</v>
+        <v>2.633709960257724</v>
       </c>
     </row>
     <row r="255" spans="1:6">
       <c r="A255" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="B255">
-        <v>0.530876880886578</v>
-      </c>
-      <c r="C255">
-        <v>1.087504894722401</v>
-      </c>
-      <c r="D255">
-        <v>0.8342258685593443</v>
-      </c>
-      <c r="E255">
-        <v>1.18266689604518</v>
+      <c r="B255" t="s">
+        <v>310</v>
+      </c>
+      <c r="C255" t="s">
+        <v>310</v>
+      </c>
+      <c r="D255" t="s">
+        <v>310</v>
+      </c>
+      <c r="E255" t="s">
+        <v>310</v>
       </c>
       <c r="F255">
-        <v>-13.50329266216636</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="256" spans="1:6">
@@ -6154,19 +6154,19 @@
         <v>260</v>
       </c>
       <c r="B256">
-        <v>0.3142289891602239</v>
+        <v>0.2986172571689287</v>
       </c>
       <c r="C256">
-        <v>0.4712087063709769</v>
+        <v>0.6770041626282567</v>
       </c>
       <c r="D256">
-        <v>0.4252895121745321</v>
+        <v>0.4583400930627415</v>
       </c>
       <c r="E256">
-        <v>0.2220376449598096</v>
+        <v>0.458334636215987</v>
       </c>
       <c r="F256">
-        <v>3.208604286000968</v>
+        <v>28.36392598371951</v>
       </c>
     </row>
     <row r="257" spans="1:6">
@@ -6242,19 +6242,19 @@
         <v>265</v>
       </c>
       <c r="B261">
-        <v>0.1960899659766658</v>
+        <v>0.2227274753774776</v>
       </c>
       <c r="C261">
-        <v>0.4248502379714472</v>
+        <v>0.4158464586045293</v>
       </c>
       <c r="D261">
-        <v>0.2892700289671046</v>
+        <v>0.3097832165182406</v>
       </c>
       <c r="E261">
-        <v>0.1804977247043953</v>
+        <v>0.1729282771339286</v>
       </c>
       <c r="F261">
-        <v>34.85277487505736</v>
+        <v>14.59371477764133</v>
       </c>
     </row>
     <row r="262" spans="1:6">
@@ -6325,7 +6325,7 @@
         <v>310</v>
       </c>
       <c r="F265">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="266" spans="1:6">
@@ -6345,7 +6345,7 @@
         <v>310</v>
       </c>
       <c r="F266">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="267" spans="1:6">
@@ -6353,19 +6353,19 @@
         <v>271</v>
       </c>
       <c r="B267">
-        <v>0.3346765879736905</v>
+        <v>0.3315890798775183</v>
       </c>
       <c r="C267">
-        <v>0.5353014379089119</v>
+        <v>0.5365151221361314</v>
       </c>
       <c r="D267">
-        <v>0.4650654058829956</v>
+        <v>0.4626110331763978</v>
       </c>
       <c r="E267">
-        <v>0.2865476294273487</v>
+        <v>0.2878484762807479</v>
       </c>
       <c r="F267">
-        <v>10.84277032568204</v>
+        <v>12.80776337492403</v>
       </c>
     </row>
     <row r="268" spans="1:6">
@@ -6373,19 +6373,19 @@
         <v>272</v>
       </c>
       <c r="B268">
-        <v>0.3921675646110954</v>
+        <v>0.36567904187651</v>
       </c>
       <c r="C268">
-        <v>0.5526793710274629</v>
+        <v>0.651757531236173</v>
       </c>
       <c r="D268">
-        <v>0.464757323476407</v>
+        <v>0.4474887793714843</v>
       </c>
       <c r="E268">
-        <v>0.3054544871593119</v>
+        <v>0.424787879523071</v>
       </c>
       <c r="F268">
-        <v>-34.89787027795651</v>
+        <v>-18.55206306972921</v>
       </c>
     </row>
     <row r="269" spans="1:6">
@@ -6410,19 +6410,19 @@
         <v>274</v>
       </c>
       <c r="B270">
-        <v>0.4046187202955151</v>
+        <v>0.4043567894480969</v>
       </c>
       <c r="C270">
-        <v>0.6640506320270375</v>
+        <v>0.6638968374532936</v>
       </c>
       <c r="D270">
-        <v>0.4903530030150812</v>
+        <v>0.4901085758385605</v>
       </c>
       <c r="E270">
-        <v>0.440963241895508</v>
+        <v>0.4407590107804851</v>
       </c>
       <c r="F270">
-        <v>-18.56620056196713</v>
+        <v>-18.53257756134921</v>
       </c>
     </row>
     <row r="271" spans="1:6">
@@ -6498,19 +6498,19 @@
         <v>279</v>
       </c>
       <c r="B275">
-        <v>1.009773703912692</v>
+        <v>0.6506929005517303</v>
       </c>
       <c r="C275">
-        <v>2.208788265519517</v>
+        <v>1.53945189991824</v>
       </c>
       <c r="D275">
-        <v>1.851478871195404</v>
+        <v>1.291747864523378</v>
       </c>
       <c r="E275">
-        <v>4.878745601896716</v>
+        <v>2.369912152161879</v>
       </c>
       <c r="F275">
-        <v>-55.0718967676006</v>
+        <v>35.1398011746773</v>
       </c>
     </row>
     <row r="276" spans="1:6">
@@ -6518,19 +6518,19 @@
         <v>280</v>
       </c>
       <c r="B276">
-        <v>0.4213977158719142</v>
+        <v>0.4267895682761799</v>
       </c>
       <c r="C276">
-        <v>0.7178397838114037</v>
+        <v>0.7058569920882536</v>
       </c>
       <c r="D276">
-        <v>0.6081930748740892</v>
+        <v>0.6051976971027392</v>
       </c>
       <c r="E276">
-        <v>0.5152939552224028</v>
+        <v>0.4982340932798768</v>
       </c>
       <c r="F276">
-        <v>1.371160247065148</v>
+        <v>0.8725454588222751</v>
       </c>
     </row>
     <row r="277" spans="1:6">
@@ -6538,19 +6538,19 @@
         <v>281</v>
       </c>
       <c r="B277">
-        <v>0.2310377107018779</v>
+        <v>0.2559645621065804</v>
       </c>
       <c r="C277">
-        <v>0.4881267785588768</v>
+        <v>0.4890333526453988</v>
       </c>
       <c r="D277">
-        <v>0.3399521357886724</v>
+        <v>0.3623847619887256</v>
       </c>
       <c r="E277">
-        <v>0.2382677519462668</v>
+        <v>0.2391536199995989</v>
       </c>
       <c r="F277">
-        <v>2.159858639082973</v>
+        <v>1.26278955338919</v>
       </c>
     </row>
     <row r="278" spans="1:6">
@@ -6570,7 +6570,7 @@
         <v>310</v>
       </c>
       <c r="F278">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="279" spans="1:6">
@@ -6595,19 +6595,19 @@
         <v>284</v>
       </c>
       <c r="B280">
-        <v>0.4014724708207713</v>
+        <v>0.4288145753476076</v>
       </c>
       <c r="C280">
-        <v>0.5639542501682535</v>
+        <v>0.6506921061103496</v>
       </c>
       <c r="D280">
-        <v>0.4800926548504955</v>
+        <v>0.5183030661027377</v>
       </c>
       <c r="E280">
-        <v>0.318044396282837</v>
+        <v>0.4234002169543223</v>
       </c>
       <c r="F280">
-        <v>-48.6532600547232</v>
+        <v>-46.04901964618873</v>
       </c>
     </row>
     <row r="281" spans="1:6">
@@ -6615,19 +6615,19 @@
         <v>285</v>
       </c>
       <c r="B281">
-        <v>0.3281795115913126</v>
+        <v>0.4076252724089895</v>
       </c>
       <c r="C281">
-        <v>0.5172749906827743</v>
+        <v>0.8143678770729171</v>
       </c>
       <c r="D281">
-        <v>0.4577500102701085</v>
+        <v>0.6432255503669044</v>
       </c>
       <c r="E281">
-        <v>0.2675734159858643</v>
+        <v>0.66319503920825</v>
       </c>
       <c r="F281">
-        <v>25.03309133001732</v>
+        <v>168.8946824042754</v>
       </c>
     </row>
     <row r="282" spans="1:6">
@@ -6635,19 +6635,19 @@
         <v>286</v>
       </c>
       <c r="B282">
-        <v>0.3028849049879863</v>
+        <v>0.2978247696880909</v>
       </c>
       <c r="C282">
-        <v>0.538993680126489</v>
+        <v>0.5421057930472445</v>
       </c>
       <c r="D282">
-        <v>0.4139711602881105</v>
+        <v>0.4098769665927419</v>
       </c>
       <c r="E282">
-        <v>0.2905141872162959</v>
+        <v>0.2938786908553819</v>
       </c>
       <c r="F282">
-        <v>24.48385931468014</v>
+        <v>27.41225652321013</v>
       </c>
     </row>
     <row r="283" spans="1:6">
@@ -6655,19 +6655,19 @@
         <v>287</v>
       </c>
       <c r="B283">
-        <v>0.04320329372616899</v>
+        <v>0.04337036595802622</v>
       </c>
       <c r="C283">
-        <v>2.216850557561442</v>
+        <v>2.323912583135101</v>
       </c>
       <c r="D283">
-        <v>1.861156135419449</v>
+        <v>1.867839215741609</v>
       </c>
       <c r="E283">
-        <v>4.914426394560476</v>
+        <v>5.400569694053657</v>
       </c>
       <c r="F283">
-        <v>-1.268582079466999</v>
+        <v>-1.053727156954971</v>
       </c>
     </row>
     <row r="284" spans="1:6">
@@ -6675,19 +6675,19 @@
         <v>288</v>
       </c>
       <c r="B284">
-        <v>0.7651628437152951</v>
+        <v>0.6614974746420909</v>
       </c>
       <c r="C284">
-        <v>1.226745193590921</v>
+        <v>1.309667772480346</v>
       </c>
       <c r="D284">
-        <v>0.9874540064969203</v>
+        <v>1.071015894878007</v>
       </c>
       <c r="E284">
-        <v>1.504903769998427</v>
+        <v>1.715229674273632</v>
       </c>
       <c r="F284">
-        <v>-225.2846422802538</v>
+        <v>4.739680037048564</v>
       </c>
     </row>
     <row r="285" spans="1:6">
@@ -6695,19 +6695,19 @@
         <v>289</v>
       </c>
       <c r="B285">
-        <v>0.3509415901570963</v>
+        <v>0.5678057334356175</v>
       </c>
       <c r="C285">
-        <v>0.5096371696331817</v>
+        <v>0.7965611045639438</v>
       </c>
       <c r="D285">
-        <v>0.4428511743453916</v>
+        <v>0.6376302510433919</v>
       </c>
       <c r="E285">
-        <v>0.2597300446717205</v>
+        <v>0.6345095933041303</v>
       </c>
       <c r="F285">
-        <v>-12.97054813180181</v>
+        <v>-99.86362536337944</v>
       </c>
     </row>
     <row r="286" spans="1:6">
@@ -6715,19 +6715,19 @@
         <v>290</v>
       </c>
       <c r="B286">
-        <v>0.3793655258348017</v>
+        <v>0.3692699618376706</v>
       </c>
       <c r="C286">
-        <v>0.7056329629700502</v>
+        <v>0.7055353021186762</v>
       </c>
       <c r="D286">
-        <v>0.5254367738075777</v>
+        <v>0.5169185707175034</v>
       </c>
       <c r="E286">
-        <v>0.4979178784298922</v>
+        <v>0.4977800625356917</v>
       </c>
       <c r="F286">
-        <v>14.62483875300465</v>
+        <v>20.70092403726645</v>
       </c>
     </row>
     <row r="287" spans="1:6">
@@ -6752,16 +6752,16 @@
         <v>292</v>
       </c>
       <c r="B288">
-        <v>0.0944998160407565</v>
+        <v>0.08559098165390283</v>
       </c>
       <c r="C288">
-        <v>0.3532938846821936</v>
+        <v>0.3479763197742006</v>
       </c>
       <c r="D288">
-        <v>0.2776373609247278</v>
+        <v>0.2524339273267548</v>
       </c>
       <c r="E288">
-        <v>0.1248165689538351</v>
+        <v>0.1210875191235967</v>
       </c>
       <c r="F288">
         <v>4</v>
@@ -6784,7 +6784,7 @@
         <v>310</v>
       </c>
       <c r="F289">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="290" spans="1:6">
@@ -6792,19 +6792,19 @@
         <v>294</v>
       </c>
       <c r="B290">
-        <v>0.3030854391919255</v>
+        <v>0.278002189914427</v>
       </c>
       <c r="C290">
-        <v>0.592333170557792</v>
+        <v>0.4782731933240739</v>
       </c>
       <c r="D290">
-        <v>0.4223276048729106</v>
+        <v>0.3966957999649919</v>
       </c>
       <c r="E290">
-        <v>0.3508585849430463</v>
+        <v>0.228745247452407</v>
       </c>
       <c r="F290">
-        <v>11.6324586825142</v>
+        <v>20.86317996278445</v>
       </c>
     </row>
     <row r="291" spans="1:6">
@@ -6829,19 +6829,19 @@
         <v>296</v>
       </c>
       <c r="B292">
-        <v>0.8759037909455689</v>
+        <v>0.7774594035522675</v>
       </c>
       <c r="C292">
-        <v>1.131811269603088</v>
+        <v>1.026846878399809</v>
       </c>
       <c r="D292">
-        <v>1.009324989302932</v>
+        <v>0.8568420920075207</v>
       </c>
       <c r="E292">
-        <v>1.280996750000553</v>
+        <v>1.054414511679433</v>
       </c>
       <c r="F292">
-        <v>-3.769966668135057</v>
+        <v>-5.035339353349823</v>
       </c>
     </row>
     <row r="293" spans="1:6">
@@ -6861,7 +6861,7 @@
         <v>310</v>
       </c>
       <c r="F293">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="294" spans="1:6">
@@ -6881,7 +6881,7 @@
         <v>310</v>
       </c>
       <c r="F294">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="295" spans="1:6">
@@ -6889,19 +6889,19 @@
         <v>299</v>
       </c>
       <c r="B295">
-        <v>0.4953783162070357</v>
+        <v>0.3859267486680049</v>
       </c>
       <c r="C295">
-        <v>0.7537695453039832</v>
+        <v>0.6432312552668148</v>
       </c>
       <c r="D295">
-        <v>0.7303113696211709</v>
+        <v>0.6095580283608988</v>
       </c>
       <c r="E295">
-        <v>0.5681685274277736</v>
+        <v>0.4137464477521222</v>
       </c>
       <c r="F295">
-        <v>1.14702223049876</v>
+        <v>1.869991548971658</v>
       </c>
     </row>
     <row r="296" spans="1:6">
@@ -6909,19 +6909,19 @@
         <v>300</v>
       </c>
       <c r="B296">
-        <v>0.3721406885490238</v>
+        <v>0.3728770431580548</v>
       </c>
       <c r="C296">
-        <v>0.6440160874729084</v>
+        <v>0.6440121186762615</v>
       </c>
       <c r="D296">
-        <v>0.5155394794623582</v>
+        <v>0.5140055323749215</v>
       </c>
       <c r="E296">
-        <v>0.4147567209239129</v>
+        <v>0.4147516090018872</v>
       </c>
       <c r="F296">
-        <v>0.7674250946470476</v>
+        <v>0.6700179050692174</v>
       </c>
     </row>
     <row r="297" spans="1:6">
@@ -6929,19 +6929,19 @@
         <v>301</v>
       </c>
       <c r="B297">
-        <v>0.2366151135043327</v>
+        <v>0.3258130249173167</v>
       </c>
       <c r="C297">
-        <v>0.4492116986892522</v>
+        <v>0.6352206133147614</v>
       </c>
       <c r="D297">
-        <v>0.340275442318099</v>
+        <v>0.422816311084208</v>
       </c>
       <c r="E297">
-        <v>0.2017911502392835</v>
+        <v>0.4035052275799817</v>
       </c>
       <c r="F297">
-        <v>35.78018040893909</v>
+        <v>-0.5192489554410427</v>
       </c>
     </row>
     <row r="298" spans="1:6">
@@ -6949,19 +6949,19 @@
         <v>302</v>
       </c>
       <c r="B298">
-        <v>0.3562306881336383</v>
+        <v>0.3447506937338676</v>
       </c>
       <c r="C298">
-        <v>0.4805977998188669</v>
+        <v>0.4726820647362978</v>
       </c>
       <c r="D298">
-        <v>0.4433075894900759</v>
+        <v>0.4331245414071198</v>
       </c>
       <c r="E298">
-        <v>0.2309742451907357</v>
+        <v>0.2234283343233696</v>
       </c>
       <c r="F298">
-        <v>-25.93007280792496</v>
+        <v>-22.24562756269876</v>
       </c>
     </row>
     <row r="299" spans="1:6">
@@ -6969,19 +6969,19 @@
         <v>303</v>
       </c>
       <c r="B299">
-        <v>0.3008207140073175</v>
+        <v>0.3014141732288501</v>
       </c>
       <c r="C299">
-        <v>0.5175155074370399</v>
+        <v>0.5130091234503288</v>
       </c>
       <c r="D299">
-        <v>0.3962373915243537</v>
+        <v>0.4072012713306088</v>
       </c>
       <c r="E299">
-        <v>0.2678223004378169</v>
+        <v>0.2631783607432747</v>
       </c>
       <c r="F299">
-        <v>-0.2545991993362265</v>
+        <v>0.6135444113686248</v>
       </c>
     </row>
     <row r="300" spans="1:6">
@@ -6989,19 +6989,19 @@
         <v>304</v>
       </c>
       <c r="B300">
-        <v>0.3750799601380851</v>
+        <v>0.3161767350657863</v>
       </c>
       <c r="C300">
-        <v>0.7071365782253897</v>
+        <v>0.5914745116788385</v>
       </c>
       <c r="D300">
-        <v>0.5000995897640312</v>
+        <v>0.4508574383001591</v>
       </c>
       <c r="E300">
-        <v>0.5000421402643127</v>
+        <v>0.3498420979657204</v>
       </c>
       <c r="F300">
-        <v>0.001087685973268418</v>
+        <v>1.123111878596341</v>
       </c>
     </row>
     <row r="301" spans="1:6">
@@ -7021,7 +7021,7 @@
         <v>310</v>
       </c>
       <c r="F301">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="302" spans="1:6">
@@ -7041,7 +7041,7 @@
         <v>310</v>
       </c>
       <c r="F302">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="303" spans="1:6">
@@ -7049,16 +7049,16 @@
         <v>307</v>
       </c>
       <c r="B303">
-        <v>0.6666615337581026</v>
+        <v>0.66675451448887</v>
       </c>
       <c r="C303">
-        <v>1.333323067516205</v>
+        <v>1.33350902897774</v>
       </c>
       <c r="D303">
-        <v>1.333323067516205</v>
+        <v>1.33350902897774</v>
       </c>
       <c r="E303">
-        <v>1.777750402370823</v>
+        <v>1.778246330365155</v>
       </c>
       <c r="F303">
         <v>1</v>
@@ -7081,7 +7081,7 @@
         <v>310</v>
       </c>
       <c r="F304">
-        <v>0</v>
+        <v>-1000</v>
       </c>
     </row>
     <row r="305" spans="1:6">
@@ -7089,19 +7089,19 @@
         <v>309</v>
       </c>
       <c r="B305">
-        <v>0.6011897004370435</v>
+        <v>0.5504934800565154</v>
       </c>
       <c r="C305">
-        <v>0.9388869332549467</v>
+        <v>0.8628000662080222</v>
       </c>
       <c r="D305">
-        <v>0.8577215482368917</v>
+        <v>0.7850487788119567</v>
       </c>
       <c r="E305">
-        <v>0.8815086734368786</v>
+        <v>0.7444239542485676</v>
       </c>
       <c r="F305">
-        <v>1.642158039296205</v>
+        <v>2.04667996998073</v>
       </c>
     </row>
   </sheetData>

</xml_diff>